<commit_message>
add event employee imported
</commit_message>
<xml_diff>
--- a/EmployeeService.API/wwwroot/Asserts/TemplateProfile.xlsx
+++ b/EmployeeService.API/wwwroot/Asserts/TemplateProfile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HRM-SYSTEM\BE\Services\EmployeeService\EmployeeService.API\wwwroot\Asserts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A49192BC-14D6-4C87-9469-6C2133B14F0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46561D45-431F-4AB6-9838-56E83636F7B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -214,7 +214,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="97">
   <si>
     <t>Email</t>
   </si>
@@ -286,9 +286,6 @@
   </si>
   <si>
     <t xml:space="preserve">    Có gia đình</t>
-  </si>
-  <si>
-    <t>Số CMND</t>
   </si>
   <si>
     <t>Nơi cấp</t>
@@ -535,6 +532,12 @@
   <si>
     <t>Đội 8 - Nghĩa Trung - Nghĩa Hưng - Nam Định - Việt Nam</t>
   </si>
+  <si>
+    <t>Mã nhân viên</t>
+  </si>
+  <si>
+    <t>Ngày gia nhập</t>
+  </si>
 </sst>
 </file>
 
@@ -1595,131 +1598,140 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1780,33 +1792,9 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1816,15 +1804,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1837,80 +1816,125 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1929,27 +1953,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2531,7 +2534,7 @@
   <dimension ref="A1:AX232"/>
   <sheetViews>
     <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+      <selection activeCell="K6" sqref="K6:N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2567,74 +2570,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:50" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="86" t="s">
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="89" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="87"/>
-      <c r="O1" s="87"/>
-      <c r="P1" s="87"/>
-      <c r="Q1" s="87"/>
-      <c r="R1" s="87"/>
-      <c r="S1" s="87"/>
-      <c r="T1" s="87"/>
-      <c r="U1" s="87"/>
-      <c r="V1" s="87"/>
-      <c r="W1" s="87"/>
-      <c r="X1" s="87"/>
-      <c r="Y1" s="87"/>
-      <c r="Z1" s="87"/>
-      <c r="AA1" s="87"/>
-      <c r="AB1" s="87"/>
-      <c r="AC1" s="87"/>
-      <c r="AD1" s="88"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="90"/>
+      <c r="K1" s="90"/>
+      <c r="L1" s="90"/>
+      <c r="M1" s="90"/>
+      <c r="N1" s="90"/>
+      <c r="O1" s="90"/>
+      <c r="P1" s="90"/>
+      <c r="Q1" s="90"/>
+      <c r="R1" s="90"/>
+      <c r="S1" s="90"/>
+      <c r="T1" s="90"/>
+      <c r="U1" s="90"/>
+      <c r="V1" s="90"/>
+      <c r="W1" s="90"/>
+      <c r="X1" s="90"/>
+      <c r="Y1" s="90"/>
+      <c r="Z1" s="90"/>
+      <c r="AA1" s="90"/>
+      <c r="AB1" s="90"/>
+      <c r="AC1" s="90"/>
+      <c r="AD1" s="91"/>
     </row>
     <row r="2" spans="1:50" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="92" t="s">
+      <c r="A2" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="93"/>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="94"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="M2" s="90"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="90"/>
-      <c r="P2" s="90"/>
-      <c r="Q2" s="90"/>
-      <c r="R2" s="90"/>
-      <c r="S2" s="90"/>
-      <c r="T2" s="90"/>
-      <c r="U2" s="90"/>
-      <c r="V2" s="90"/>
-      <c r="W2" s="90"/>
-      <c r="X2" s="90"/>
-      <c r="Y2" s="90"/>
-      <c r="Z2" s="90"/>
-      <c r="AA2" s="90"/>
-      <c r="AB2" s="90"/>
-      <c r="AC2" s="90"/>
-      <c r="AD2" s="91"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="93"/>
+      <c r="K2" s="93"/>
+      <c r="L2" s="93"/>
+      <c r="M2" s="93"/>
+      <c r="N2" s="93"/>
+      <c r="O2" s="93"/>
+      <c r="P2" s="93"/>
+      <c r="Q2" s="93"/>
+      <c r="R2" s="93"/>
+      <c r="S2" s="93"/>
+      <c r="T2" s="93"/>
+      <c r="U2" s="93"/>
+      <c r="V2" s="93"/>
+      <c r="W2" s="93"/>
+      <c r="X2" s="93"/>
+      <c r="Y2" s="93"/>
+      <c r="Z2" s="93"/>
+      <c r="AA2" s="93"/>
+      <c r="AB2" s="93"/>
+      <c r="AC2" s="93"/>
+      <c r="AD2" s="94"/>
     </row>
     <row r="3" spans="1:50" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
@@ -2644,57 +2647,57 @@
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
       <c r="G3" s="14"/>
-      <c r="H3" s="95" t="s">
+      <c r="H3" s="98" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="97" t="s">
-        <v>72</v>
-      </c>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
-      <c r="O3" s="98"/>
-      <c r="P3" s="98"/>
-      <c r="Q3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="100" t="s">
+        <v>71</v>
+      </c>
+      <c r="L3" s="101"/>
+      <c r="M3" s="101"/>
+      <c r="N3" s="101"/>
+      <c r="O3" s="101"/>
+      <c r="P3" s="101"/>
+      <c r="Q3" s="102"/>
       <c r="R3" s="15" t="s">
         <v>15</v>
       </c>
       <c r="S3" s="15"/>
-      <c r="T3" s="100" t="s">
-        <v>65</v>
-      </c>
-      <c r="U3" s="101"/>
-      <c r="V3" s="101"/>
-      <c r="W3" s="102"/>
-      <c r="X3" s="96" t="s">
+      <c r="T3" s="103" t="s">
+        <v>64</v>
+      </c>
+      <c r="U3" s="104"/>
+      <c r="V3" s="104"/>
+      <c r="W3" s="105"/>
+      <c r="X3" s="99" t="s">
         <v>16</v>
       </c>
-      <c r="Y3" s="96"/>
-      <c r="Z3" s="96"/>
-      <c r="AA3" s="112" t="s">
+      <c r="Y3" s="99"/>
+      <c r="Z3" s="99"/>
+      <c r="AA3" s="109" t="s">
         <v>18</v>
       </c>
-      <c r="AB3" s="112"/>
-      <c r="AC3" s="100" t="s">
+      <c r="AB3" s="109"/>
+      <c r="AC3" s="103" t="s">
         <v>17</v>
       </c>
-      <c r="AD3" s="117"/>
+      <c r="AD3" s="112"/>
     </row>
     <row r="4" spans="1:50" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
-      <c r="B4" s="129"/>
-      <c r="C4" s="130"/>
-      <c r="D4" s="130"/>
-      <c r="E4" s="130"/>
-      <c r="F4" s="131"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="52"/>
       <c r="G4" s="14"/>
-      <c r="H4" s="121" t="s">
-        <v>50</v>
-      </c>
-      <c r="I4" s="44"/>
-      <c r="J4" s="44"/>
+      <c r="H4" s="113" t="s">
+        <v>49</v>
+      </c>
+      <c r="I4" s="75"/>
+      <c r="J4" s="75"/>
       <c r="K4" s="35">
         <v>7</v>
       </c>
@@ -2704,16 +2707,16 @@
       <c r="M4" s="40">
         <v>2003</v>
       </c>
-      <c r="N4" s="139" t="s">
+      <c r="N4" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="O4" s="140"/>
-      <c r="P4" s="122" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q4" s="123"/>
-      <c r="R4" s="123"/>
-      <c r="S4" s="124"/>
+      <c r="O4" s="62"/>
+      <c r="P4" s="114" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q4" s="115"/>
+      <c r="R4" s="115"/>
+      <c r="S4" s="116"/>
       <c r="T4" s="22" t="s">
         <v>21</v>
       </c>
@@ -2725,11 +2728,11 @@
       </c>
       <c r="Y4" s="3"/>
       <c r="Z4" s="7"/>
-      <c r="AA4" s="43" t="s">
+      <c r="AA4" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="AB4" s="44"/>
-      <c r="AC4" s="45"/>
+      <c r="AB4" s="75"/>
+      <c r="AC4" s="80"/>
       <c r="AD4" s="26" t="e">
         <f>K4&amp;"/"&amp;#REF!&amp;"/"&amp;L4</f>
         <v>#REF!</v>
@@ -2738,69 +2741,69 @@
     </row>
     <row r="5" spans="1:50" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
-      <c r="B5" s="132"/>
-      <c r="C5" s="133"/>
-      <c r="D5" s="133"/>
-      <c r="E5" s="133"/>
-      <c r="F5" s="134"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="55"/>
       <c r="G5" s="14"/>
-      <c r="H5" s="138" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5" s="114"/>
-      <c r="J5" s="114"/>
-      <c r="K5" s="118"/>
-      <c r="L5" s="119"/>
-      <c r="M5" s="119"/>
-      <c r="N5" s="120"/>
-      <c r="O5" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="P5" s="44"/>
+      <c r="H5" s="59" t="s">
+        <v>95</v>
+      </c>
+      <c r="I5" s="60"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="71"/>
+      <c r="L5" s="72"/>
+      <c r="M5" s="72"/>
+      <c r="N5" s="73"/>
+      <c r="O5" s="74" t="s">
+        <v>96</v>
+      </c>
+      <c r="P5" s="75"/>
       <c r="Q5" s="40"/>
       <c r="R5" s="40"/>
       <c r="S5" s="40"/>
-      <c r="T5" s="44" t="s">
+      <c r="T5" s="75" t="s">
+        <v>24</v>
+      </c>
+      <c r="U5" s="76"/>
+      <c r="V5" s="63"/>
+      <c r="W5" s="64"/>
+      <c r="X5" s="65"/>
+      <c r="Y5" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="U5" s="41"/>
-      <c r="V5" s="141"/>
-      <c r="W5" s="142"/>
-      <c r="X5" s="143"/>
-      <c r="Y5" s="109" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z5" s="110"/>
-      <c r="AA5" s="111"/>
-      <c r="AB5" s="113">
+      <c r="Z5" s="78"/>
+      <c r="AA5" s="79"/>
+      <c r="AB5" s="49">
         <v>3620719324</v>
       </c>
-      <c r="AC5" s="107"/>
-      <c r="AD5" s="108"/>
+      <c r="AC5" s="41"/>
+      <c r="AD5" s="42"/>
     </row>
     <row r="6" spans="1:50" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
-      <c r="B6" s="132"/>
-      <c r="C6" s="133"/>
-      <c r="D6" s="133"/>
-      <c r="E6" s="133"/>
-      <c r="F6" s="134"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="55"/>
       <c r="G6" s="14"/>
-      <c r="H6" s="138" t="s">
-        <v>71</v>
-      </c>
-      <c r="I6" s="114"/>
-      <c r="J6" s="114"/>
-      <c r="K6" s="118">
+      <c r="H6" s="59" t="s">
+        <v>70</v>
+      </c>
+      <c r="I6" s="60"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="71">
         <v>36203001326</v>
       </c>
-      <c r="L6" s="119"/>
-      <c r="M6" s="119"/>
-      <c r="N6" s="120"/>
-      <c r="O6" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="P6" s="44"/>
+      <c r="L6" s="72"/>
+      <c r="M6" s="72"/>
+      <c r="N6" s="73"/>
+      <c r="O6" s="74" t="s">
+        <v>50</v>
+      </c>
+      <c r="P6" s="75"/>
       <c r="Q6" s="40">
         <v>25</v>
       </c>
@@ -2810,21 +2813,21 @@
       <c r="S6" s="40">
         <v>2021</v>
       </c>
-      <c r="T6" s="44" t="s">
-        <v>25</v>
-      </c>
-      <c r="U6" s="41"/>
-      <c r="V6" s="141" t="s">
-        <v>74</v>
-      </c>
-      <c r="W6" s="142"/>
-      <c r="X6" s="143"/>
-      <c r="Y6" s="109"/>
-      <c r="Z6" s="110"/>
-      <c r="AA6" s="111"/>
-      <c r="AB6" s="113"/>
-      <c r="AC6" s="107"/>
-      <c r="AD6" s="108"/>
+      <c r="T6" s="75" t="s">
+        <v>24</v>
+      </c>
+      <c r="U6" s="76"/>
+      <c r="V6" s="63" t="s">
+        <v>73</v>
+      </c>
+      <c r="W6" s="64"/>
+      <c r="X6" s="65"/>
+      <c r="Y6" s="77"/>
+      <c r="Z6" s="78"/>
+      <c r="AA6" s="79"/>
+      <c r="AB6" s="49"/>
+      <c r="AC6" s="41"/>
+      <c r="AD6" s="42"/>
       <c r="AE6" s="26" t="e">
         <f>Q6&amp;"/"&amp;#REF!&amp;"/"&amp;S6</f>
         <v>#REF!</v>
@@ -2832,125 +2835,125 @@
     </row>
     <row r="7" spans="1:50" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
-      <c r="B7" s="132"/>
-      <c r="C7" s="133"/>
-      <c r="D7" s="133"/>
-      <c r="E7" s="133"/>
-      <c r="F7" s="134"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="55"/>
       <c r="G7" s="14"/>
       <c r="H7" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I7" s="17"/>
       <c r="J7" s="17"/>
-      <c r="K7" s="103" t="s">
-        <v>95</v>
-      </c>
-      <c r="L7" s="104"/>
-      <c r="M7" s="104"/>
-      <c r="N7" s="104"/>
-      <c r="O7" s="104"/>
-      <c r="P7" s="104"/>
-      <c r="Q7" s="104"/>
-      <c r="R7" s="104"/>
-      <c r="S7" s="104"/>
-      <c r="T7" s="104"/>
-      <c r="U7" s="104"/>
-      <c r="V7" s="104"/>
-      <c r="W7" s="104"/>
-      <c r="X7" s="105"/>
-      <c r="Y7" s="114" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z7" s="114"/>
-      <c r="AA7" s="114"/>
-      <c r="AB7" s="115">
+      <c r="K7" s="106" t="s">
+        <v>94</v>
+      </c>
+      <c r="L7" s="107"/>
+      <c r="M7" s="107"/>
+      <c r="N7" s="107"/>
+      <c r="O7" s="107"/>
+      <c r="P7" s="107"/>
+      <c r="Q7" s="107"/>
+      <c r="R7" s="107"/>
+      <c r="S7" s="107"/>
+      <c r="T7" s="107"/>
+      <c r="U7" s="107"/>
+      <c r="V7" s="107"/>
+      <c r="W7" s="107"/>
+      <c r="X7" s="108"/>
+      <c r="Y7" s="60" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z7" s="60"/>
+      <c r="AA7" s="60"/>
+      <c r="AB7" s="110">
         <v>919434401</v>
       </c>
-      <c r="AC7" s="114"/>
-      <c r="AD7" s="116"/>
+      <c r="AC7" s="60"/>
+      <c r="AD7" s="111"/>
     </row>
     <row r="8" spans="1:50" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
-      <c r="B8" s="132"/>
-      <c r="C8" s="133"/>
-      <c r="D8" s="133"/>
-      <c r="E8" s="133"/>
-      <c r="F8" s="134"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="55"/>
       <c r="G8" s="14"/>
       <c r="H8" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="6"/>
-      <c r="K8" s="103" t="s">
-        <v>75</v>
-      </c>
-      <c r="L8" s="104"/>
-      <c r="M8" s="104"/>
-      <c r="N8" s="104"/>
-      <c r="O8" s="104"/>
-      <c r="P8" s="104"/>
-      <c r="Q8" s="104"/>
-      <c r="R8" s="104"/>
-      <c r="S8" s="104"/>
-      <c r="T8" s="104"/>
-      <c r="U8" s="104"/>
-      <c r="V8" s="104"/>
-      <c r="W8" s="104"/>
-      <c r="X8" s="105"/>
+      <c r="K8" s="106" t="s">
+        <v>74</v>
+      </c>
+      <c r="L8" s="107"/>
+      <c r="M8" s="107"/>
+      <c r="N8" s="107"/>
+      <c r="O8" s="107"/>
+      <c r="P8" s="107"/>
+      <c r="Q8" s="107"/>
+      <c r="R8" s="107"/>
+      <c r="S8" s="107"/>
+      <c r="T8" s="107"/>
+      <c r="U8" s="107"/>
+      <c r="V8" s="107"/>
+      <c r="W8" s="107"/>
+      <c r="X8" s="108"/>
       <c r="Y8" s="17" t="s">
         <v>0</v>
       </c>
       <c r="Z8" s="17"/>
-      <c r="AA8" s="106" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB8" s="107"/>
-      <c r="AC8" s="107"/>
-      <c r="AD8" s="108"/>
+      <c r="AA8" s="66" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB8" s="41"/>
+      <c r="AC8" s="41"/>
+      <c r="AD8" s="42"/>
     </row>
     <row r="9" spans="1:50" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
-      <c r="B9" s="135"/>
-      <c r="C9" s="136"/>
-      <c r="D9" s="136"/>
-      <c r="E9" s="136"/>
-      <c r="F9" s="137"/>
+      <c r="B9" s="56"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="58"/>
       <c r="G9" s="14"/>
       <c r="H9" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I9" s="17"/>
       <c r="J9" s="17"/>
-      <c r="K9" s="149">
+      <c r="K9" s="82">
         <v>45547</v>
       </c>
-      <c r="L9" s="44"/>
-      <c r="M9" s="44"/>
-      <c r="N9" s="44"/>
-      <c r="O9" s="41"/>
+      <c r="L9" s="75"/>
+      <c r="M9" s="75"/>
+      <c r="N9" s="75"/>
+      <c r="O9" s="76"/>
       <c r="P9" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q9" s="148" t="s">
-        <v>76</v>
-      </c>
-      <c r="R9" s="44"/>
-      <c r="S9" s="44"/>
-      <c r="T9" s="44"/>
-      <c r="U9" s="44"/>
-      <c r="V9" s="44"/>
-      <c r="W9" s="44"/>
-      <c r="X9" s="41"/>
+        <v>68</v>
+      </c>
+      <c r="Q9" s="81" t="s">
+        <v>75</v>
+      </c>
+      <c r="R9" s="75"/>
+      <c r="S9" s="75"/>
+      <c r="T9" s="75"/>
+      <c r="U9" s="75"/>
+      <c r="V9" s="75"/>
+      <c r="W9" s="75"/>
+      <c r="X9" s="76"/>
       <c r="Y9" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Z9" s="25"/>
-      <c r="AA9" s="106"/>
-      <c r="AB9" s="107"/>
-      <c r="AC9" s="107"/>
-      <c r="AD9" s="108"/>
+      <c r="AA9" s="66"/>
+      <c r="AB9" s="41"/>
+      <c r="AC9" s="41"/>
+      <c r="AD9" s="42"/>
     </row>
     <row r="10" spans="1:50" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="19"/>
@@ -2961,47 +2964,47 @@
       <c r="F10" s="20"/>
       <c r="G10" s="21"/>
       <c r="H10" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I10" s="17"/>
       <c r="J10" s="17"/>
       <c r="K10" s="17"/>
       <c r="L10" s="22"/>
       <c r="M10" s="10"/>
-      <c r="N10" s="144" t="s">
-        <v>78</v>
-      </c>
-      <c r="O10" s="145"/>
-      <c r="P10" s="145"/>
-      <c r="Q10" s="146"/>
-      <c r="R10" s="146"/>
-      <c r="S10" s="146"/>
-      <c r="T10" s="146"/>
-      <c r="U10" s="147"/>
-      <c r="V10" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="W10" s="44"/>
-      <c r="X10" s="44"/>
-      <c r="Y10" s="44"/>
-      <c r="Z10" s="41"/>
-      <c r="AA10" s="113">
+      <c r="N10" s="67" t="s">
+        <v>77</v>
+      </c>
+      <c r="O10" s="68"/>
+      <c r="P10" s="68"/>
+      <c r="Q10" s="69"/>
+      <c r="R10" s="69"/>
+      <c r="S10" s="69"/>
+      <c r="T10" s="69"/>
+      <c r="U10" s="70"/>
+      <c r="V10" s="74" t="s">
+        <v>31</v>
+      </c>
+      <c r="W10" s="75"/>
+      <c r="X10" s="75"/>
+      <c r="Y10" s="75"/>
+      <c r="Z10" s="76"/>
+      <c r="AA10" s="49">
         <v>917422097</v>
       </c>
-      <c r="AB10" s="107"/>
-      <c r="AC10" s="107"/>
-      <c r="AD10" s="108"/>
+      <c r="AB10" s="41"/>
+      <c r="AC10" s="41"/>
+      <c r="AD10" s="42"/>
     </row>
     <row r="11" spans="1:50" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="126" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="127"/>
-      <c r="C11" s="127"/>
-      <c r="D11" s="127"/>
-      <c r="E11" s="127"/>
-      <c r="F11" s="127"/>
-      <c r="G11" s="128"/>
+      <c r="A11" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="45"/>
       <c r="H11" s="46">
         <v>8649605034</v>
       </c>
@@ -3009,47 +3012,47 @@
       <c r="J11" s="47"/>
       <c r="K11" s="47"/>
       <c r="L11" s="47"/>
-      <c r="M11" s="50"/>
-      <c r="N11" s="43" t="s">
-        <v>70</v>
-      </c>
-      <c r="O11" s="44"/>
-      <c r="P11" s="44"/>
-      <c r="Q11" s="44"/>
-      <c r="R11" s="44"/>
-      <c r="S11" s="44"/>
-      <c r="T11" s="44"/>
-      <c r="U11" s="107"/>
-      <c r="V11" s="107"/>
-      <c r="W11" s="107"/>
-      <c r="X11" s="107"/>
-      <c r="Y11" s="107"/>
-      <c r="Z11" s="107"/>
-      <c r="AA11" s="107"/>
-      <c r="AB11" s="107"/>
-      <c r="AC11" s="107"/>
-      <c r="AD11" s="108"/>
+      <c r="M11" s="48"/>
+      <c r="N11" s="74" t="s">
+        <v>69</v>
+      </c>
+      <c r="O11" s="75"/>
+      <c r="P11" s="75"/>
+      <c r="Q11" s="75"/>
+      <c r="R11" s="75"/>
+      <c r="S11" s="75"/>
+      <c r="T11" s="75"/>
+      <c r="U11" s="41"/>
+      <c r="V11" s="41"/>
+      <c r="W11" s="41"/>
+      <c r="X11" s="41"/>
+      <c r="Y11" s="41"/>
+      <c r="Z11" s="41"/>
+      <c r="AA11" s="41"/>
+      <c r="AB11" s="41"/>
+      <c r="AC11" s="41"/>
+      <c r="AD11" s="42"/>
     </row>
     <row r="12" spans="1:50" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="69" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="70"/>
-      <c r="C12" s="70"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="70"/>
-      <c r="G12" s="71"/>
+      <c r="A12" s="132" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="133"/>
+      <c r="C12" s="133"/>
+      <c r="D12" s="133"/>
+      <c r="E12" s="133"/>
+      <c r="F12" s="133"/>
+      <c r="G12" s="134"/>
       <c r="H12" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I12" s="47"/>
       <c r="J12" s="47"/>
       <c r="K12" s="47"/>
       <c r="L12" s="47"/>
-      <c r="M12" s="50"/>
+      <c r="M12" s="48"/>
       <c r="N12" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O12" s="5"/>
       <c r="P12" s="46">
@@ -3058,99 +3061,99 @@
       <c r="Q12" s="47"/>
       <c r="R12" s="47"/>
       <c r="S12" s="47"/>
-      <c r="T12" s="50"/>
+      <c r="T12" s="48"/>
       <c r="U12" s="46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="V12" s="47"/>
       <c r="W12" s="47"/>
       <c r="X12" s="47"/>
       <c r="Y12" s="47" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Z12" s="47"/>
       <c r="AA12" s="47"/>
       <c r="AB12" s="47"/>
       <c r="AC12" s="47"/>
-      <c r="AD12" s="48"/>
+      <c r="AD12" s="83"/>
     </row>
     <row r="13" spans="1:50" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="125" t="s">
+      <c r="A13" s="85" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="85"/>
+      <c r="C13" s="85"/>
+      <c r="D13" s="85"/>
+      <c r="E13" s="85"/>
+      <c r="F13" s="85"/>
+      <c r="G13" s="85"/>
+      <c r="H13" s="85" t="s">
+        <v>78</v>
+      </c>
+      <c r="I13" s="85"/>
+      <c r="J13" s="85"/>
+      <c r="K13" s="85"/>
+      <c r="L13" s="85"/>
+      <c r="M13" s="85"/>
+      <c r="N13" s="142" t="s">
         <v>66</v>
       </c>
-      <c r="B13" s="125"/>
-      <c r="C13" s="125"/>
-      <c r="D13" s="125"/>
-      <c r="E13" s="125"/>
-      <c r="F13" s="125"/>
-      <c r="G13" s="125"/>
-      <c r="H13" s="125" t="s">
+      <c r="O13" s="142"/>
+      <c r="P13" s="142"/>
+      <c r="Q13" s="142"/>
+      <c r="R13" s="142"/>
+      <c r="S13" s="142"/>
+      <c r="T13" s="142"/>
+      <c r="U13" s="142" t="s">
         <v>79</v>
       </c>
-      <c r="I13" s="125"/>
-      <c r="J13" s="125"/>
-      <c r="K13" s="125"/>
-      <c r="L13" s="125"/>
-      <c r="M13" s="125"/>
-      <c r="N13" s="75" t="s">
-        <v>67</v>
-      </c>
-      <c r="O13" s="75"/>
-      <c r="P13" s="75"/>
-      <c r="Q13" s="75"/>
-      <c r="R13" s="75"/>
-      <c r="S13" s="75"/>
-      <c r="T13" s="75"/>
-      <c r="U13" s="75" t="s">
-        <v>80</v>
-      </c>
-      <c r="V13" s="75"/>
-      <c r="W13" s="75"/>
-      <c r="X13" s="75"/>
-      <c r="Y13" s="75"/>
-      <c r="Z13" s="75"/>
-      <c r="AA13" s="75"/>
-      <c r="AB13" s="75"/>
-      <c r="AC13" s="75"/>
-      <c r="AD13" s="75"/>
+      <c r="V13" s="142"/>
+      <c r="W13" s="142"/>
+      <c r="X13" s="142"/>
+      <c r="Y13" s="142"/>
+      <c r="Z13" s="142"/>
+      <c r="AA13" s="142"/>
+      <c r="AB13" s="142"/>
+      <c r="AC13" s="142"/>
+      <c r="AD13" s="142"/>
     </row>
     <row r="14" spans="1:50" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="72" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="73"/>
-      <c r="C14" s="74" t="s">
+      <c r="A14" s="135" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="136"/>
+      <c r="C14" s="141" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="128"/>
+      <c r="E14" s="128"/>
+      <c r="F14" s="128" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="128"/>
+      <c r="H14" s="128"/>
+      <c r="I14" s="128"/>
+      <c r="J14" s="128"/>
+      <c r="K14" s="128" t="s">
+        <v>19</v>
+      </c>
+      <c r="L14" s="128"/>
+      <c r="M14" s="128"/>
+      <c r="N14" s="128"/>
+      <c r="O14" s="129" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="65"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="65" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" s="65"/>
-      <c r="H14" s="65"/>
-      <c r="I14" s="65"/>
-      <c r="J14" s="65"/>
-      <c r="K14" s="65" t="s">
-        <v>19</v>
-      </c>
-      <c r="L14" s="65"/>
-      <c r="M14" s="65"/>
-      <c r="N14" s="65"/>
-      <c r="O14" s="66" t="s">
-        <v>36</v>
-      </c>
-      <c r="P14" s="67"/>
-      <c r="Q14" s="67"/>
-      <c r="R14" s="67"/>
-      <c r="S14" s="67"/>
-      <c r="T14" s="67"/>
-      <c r="U14" s="68"/>
+      <c r="P14" s="130"/>
+      <c r="Q14" s="130"/>
+      <c r="R14" s="130"/>
+      <c r="S14" s="130"/>
+      <c r="T14" s="130"/>
+      <c r="U14" s="131"/>
       <c r="V14" s="36"/>
       <c r="W14" s="36"/>
       <c r="X14" s="37"/>
       <c r="Y14" s="38" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Z14" s="36"/>
       <c r="AA14" s="36"/>
@@ -3159,95 +3162,95 @@
       <c r="AD14" s="39"/>
     </row>
     <row r="15" spans="1:50" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="59"/>
-      <c r="B15" s="60"/>
-      <c r="C15" s="78" t="s">
+      <c r="A15" s="137"/>
+      <c r="B15" s="138"/>
+      <c r="C15" s="123" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="124"/>
+      <c r="E15" s="124"/>
+      <c r="F15" s="124" t="s">
+        <v>83</v>
+      </c>
+      <c r="G15" s="124"/>
+      <c r="H15" s="124"/>
+      <c r="I15" s="124"/>
+      <c r="J15" s="124"/>
+      <c r="K15" s="125">
+        <v>29221</v>
+      </c>
+      <c r="L15" s="124"/>
+      <c r="M15" s="124"/>
+      <c r="N15" s="124"/>
+      <c r="O15" s="119" t="s">
+        <v>72</v>
+      </c>
+      <c r="P15" s="120"/>
+      <c r="Q15" s="120"/>
+      <c r="R15" s="120"/>
+      <c r="S15" s="120"/>
+      <c r="T15" s="120"/>
+      <c r="U15" s="121"/>
+      <c r="V15" s="119" t="s">
+        <v>72</v>
+      </c>
+      <c r="W15" s="120"/>
+      <c r="X15" s="120"/>
+      <c r="Y15" s="120"/>
+      <c r="Z15" s="120"/>
+      <c r="AA15" s="120"/>
+      <c r="AB15" s="120"/>
+      <c r="AC15" s="120"/>
+      <c r="AD15" s="122"/>
+    </row>
+    <row r="16" spans="1:50" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="137"/>
+      <c r="B16" s="138"/>
+      <c r="C16" s="84" t="s">
         <v>81</v>
       </c>
-      <c r="D15" s="79"/>
-      <c r="E15" s="79"/>
-      <c r="F15" s="79" t="s">
+      <c r="D16" s="84"/>
+      <c r="E16" s="84"/>
+      <c r="F16" s="84" t="s">
         <v>84</v>
       </c>
-      <c r="G15" s="79"/>
-      <c r="H15" s="79"/>
-      <c r="I15" s="79"/>
-      <c r="J15" s="79"/>
-      <c r="K15" s="80">
-        <v>29221</v>
-      </c>
-      <c r="L15" s="79"/>
-      <c r="M15" s="79"/>
-      <c r="N15" s="79"/>
-      <c r="O15" s="53" t="s">
-        <v>73</v>
-      </c>
-      <c r="P15" s="54"/>
-      <c r="Q15" s="54"/>
-      <c r="R15" s="54"/>
-      <c r="S15" s="54"/>
-      <c r="T15" s="54"/>
-      <c r="U15" s="55"/>
-      <c r="V15" s="53" t="s">
-        <v>73</v>
-      </c>
-      <c r="W15" s="54"/>
-      <c r="X15" s="54"/>
-      <c r="Y15" s="54"/>
-      <c r="Z15" s="54"/>
-      <c r="AA15" s="54"/>
-      <c r="AB15" s="54"/>
-      <c r="AC15" s="54"/>
-      <c r="AD15" s="56"/>
-    </row>
-    <row r="16" spans="1:50" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="59"/>
-      <c r="B16" s="60"/>
-      <c r="C16" s="42" t="s">
-        <v>82</v>
-      </c>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
-      <c r="K16" s="77">
+      <c r="G16" s="84"/>
+      <c r="H16" s="84"/>
+      <c r="I16" s="84"/>
+      <c r="J16" s="84"/>
+      <c r="K16" s="118">
         <v>30682</v>
       </c>
-      <c r="L16" s="42"/>
-      <c r="M16" s="42"/>
-      <c r="N16" s="42"/>
-      <c r="O16" s="43" t="s">
-        <v>73</v>
-      </c>
-      <c r="P16" s="44"/>
-      <c r="Q16" s="44"/>
-      <c r="R16" s="44"/>
-      <c r="S16" s="44"/>
-      <c r="T16" s="44"/>
-      <c r="U16" s="41"/>
-      <c r="V16" s="81" t="s">
-        <v>73</v>
-      </c>
-      <c r="W16" s="82"/>
-      <c r="X16" s="82"/>
-      <c r="Y16" s="82"/>
-      <c r="Z16" s="82"/>
-      <c r="AA16" s="82"/>
-      <c r="AB16" s="82"/>
-      <c r="AC16" s="82"/>
-      <c r="AD16" s="82"/>
+      <c r="L16" s="84"/>
+      <c r="M16" s="84"/>
+      <c r="N16" s="84"/>
+      <c r="O16" s="74" t="s">
+        <v>72</v>
+      </c>
+      <c r="P16" s="75"/>
+      <c r="Q16" s="75"/>
+      <c r="R16" s="75"/>
+      <c r="S16" s="75"/>
+      <c r="T16" s="75"/>
+      <c r="U16" s="76"/>
+      <c r="V16" s="126" t="s">
+        <v>72</v>
+      </c>
+      <c r="W16" s="127"/>
+      <c r="X16" s="127"/>
+      <c r="Y16" s="127"/>
+      <c r="Z16" s="127"/>
+      <c r="AA16" s="127"/>
+      <c r="AB16" s="127"/>
+      <c r="AC16" s="127"/>
+      <c r="AD16" s="127"/>
       <c r="AE16" s="27"/>
       <c r="AF16" s="24"/>
       <c r="AG16" s="24"/>
       <c r="AH16" s="24"/>
       <c r="AI16" s="24"/>
-      <c r="AJ16" s="76"/>
-      <c r="AK16" s="76"/>
+      <c r="AJ16" s="117"/>
+      <c r="AK16" s="117"/>
       <c r="AL16" s="24"/>
       <c r="AM16" s="24"/>
       <c r="AN16" s="24"/>
@@ -3258,358 +3261,358 @@
       <c r="AS16" s="24"/>
       <c r="AT16" s="24"/>
       <c r="AU16" s="24"/>
-      <c r="AV16" s="76"/>
-      <c r="AW16" s="76"/>
-      <c r="AX16" s="76"/>
+      <c r="AV16" s="117"/>
+      <c r="AW16" s="117"/>
+      <c r="AX16" s="117"/>
     </row>
     <row r="17" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="59"/>
-      <c r="B17" s="60"/>
-      <c r="C17" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42" t="s">
+      <c r="A17" s="137"/>
+      <c r="B17" s="138"/>
+      <c r="C17" s="76" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" s="84"/>
+      <c r="E17" s="84"/>
+      <c r="F17" s="84" t="s">
+        <v>85</v>
+      </c>
+      <c r="G17" s="84"/>
+      <c r="H17" s="84"/>
+      <c r="I17" s="84"/>
+      <c r="J17" s="84"/>
+      <c r="K17" s="84" t="s">
         <v>86</v>
       </c>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
-      <c r="K17" s="42" t="s">
+      <c r="L17" s="84"/>
+      <c r="M17" s="84"/>
+      <c r="N17" s="84"/>
+      <c r="O17" s="74" t="s">
         <v>87</v>
       </c>
-      <c r="L17" s="42"/>
-      <c r="M17" s="42"/>
-      <c r="N17" s="42"/>
-      <c r="O17" s="43" t="s">
-        <v>88</v>
-      </c>
-      <c r="P17" s="44"/>
-      <c r="Q17" s="44"/>
-      <c r="R17" s="44"/>
-      <c r="S17" s="44"/>
-      <c r="T17" s="44"/>
-      <c r="U17" s="41"/>
-      <c r="V17" s="43" t="s">
-        <v>73</v>
-      </c>
-      <c r="W17" s="44"/>
-      <c r="X17" s="44"/>
-      <c r="Y17" s="44"/>
-      <c r="Z17" s="44"/>
-      <c r="AA17" s="44"/>
-      <c r="AB17" s="44"/>
-      <c r="AC17" s="44"/>
-      <c r="AD17" s="45"/>
+      <c r="P17" s="75"/>
+      <c r="Q17" s="75"/>
+      <c r="R17" s="75"/>
+      <c r="S17" s="75"/>
+      <c r="T17" s="75"/>
+      <c r="U17" s="76"/>
+      <c r="V17" s="74" t="s">
+        <v>72</v>
+      </c>
+      <c r="W17" s="75"/>
+      <c r="X17" s="75"/>
+      <c r="Y17" s="75"/>
+      <c r="Z17" s="75"/>
+      <c r="AA17" s="75"/>
+      <c r="AB17" s="75"/>
+      <c r="AC17" s="75"/>
+      <c r="AD17" s="80"/>
     </row>
     <row r="18" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="59"/>
-      <c r="B18" s="60"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
-      <c r="K18" s="42"/>
-      <c r="L18" s="42"/>
-      <c r="M18" s="42"/>
-      <c r="N18" s="42"/>
-      <c r="O18" s="42"/>
-      <c r="P18" s="42"/>
-      <c r="Q18" s="42"/>
-      <c r="R18" s="43"/>
+      <c r="A18" s="137"/>
+      <c r="B18" s="138"/>
+      <c r="C18" s="76"/>
+      <c r="D18" s="84"/>
+      <c r="E18" s="84"/>
+      <c r="F18" s="84"/>
+      <c r="G18" s="84"/>
+      <c r="H18" s="84"/>
+      <c r="I18" s="84"/>
+      <c r="J18" s="84"/>
+      <c r="K18" s="84"/>
+      <c r="L18" s="84"/>
+      <c r="M18" s="84"/>
+      <c r="N18" s="84"/>
+      <c r="O18" s="84"/>
+      <c r="P18" s="84"/>
+      <c r="Q18" s="84"/>
+      <c r="R18" s="74"/>
       <c r="S18" s="2"/>
       <c r="T18" s="2"/>
       <c r="U18" s="7"/>
       <c r="V18" s="2"/>
       <c r="W18" s="2"/>
       <c r="X18" s="2"/>
-      <c r="Y18" s="44"/>
-      <c r="Z18" s="44"/>
-      <c r="AA18" s="44"/>
-      <c r="AB18" s="44"/>
-      <c r="AC18" s="44"/>
-      <c r="AD18" s="45"/>
+      <c r="Y18" s="75"/>
+      <c r="Z18" s="75"/>
+      <c r="AA18" s="75"/>
+      <c r="AB18" s="75"/>
+      <c r="AC18" s="75"/>
+      <c r="AD18" s="80"/>
     </row>
     <row r="19" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="59"/>
-      <c r="B19" s="60"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="42"/>
-      <c r="H19" s="42"/>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
-      <c r="K19" s="42"/>
-      <c r="L19" s="42"/>
-      <c r="M19" s="42"/>
-      <c r="N19" s="42"/>
-      <c r="O19" s="42"/>
-      <c r="P19" s="42"/>
-      <c r="Q19" s="42"/>
-      <c r="R19" s="43"/>
+      <c r="A19" s="137"/>
+      <c r="B19" s="138"/>
+      <c r="C19" s="76"/>
+      <c r="D19" s="84"/>
+      <c r="E19" s="84"/>
+      <c r="F19" s="84"/>
+      <c r="G19" s="84"/>
+      <c r="H19" s="84"/>
+      <c r="I19" s="84"/>
+      <c r="J19" s="84"/>
+      <c r="K19" s="84"/>
+      <c r="L19" s="84"/>
+      <c r="M19" s="84"/>
+      <c r="N19" s="84"/>
+      <c r="O19" s="84"/>
+      <c r="P19" s="84"/>
+      <c r="Q19" s="84"/>
+      <c r="R19" s="74"/>
       <c r="S19" s="2"/>
       <c r="T19" s="2"/>
       <c r="U19" s="7"/>
       <c r="V19" s="2"/>
       <c r="W19" s="2"/>
       <c r="X19" s="2"/>
-      <c r="Y19" s="44"/>
-      <c r="Z19" s="44"/>
-      <c r="AA19" s="44"/>
-      <c r="AB19" s="44"/>
-      <c r="AC19" s="44"/>
-      <c r="AD19" s="45"/>
+      <c r="Y19" s="75"/>
+      <c r="Z19" s="75"/>
+      <c r="AA19" s="75"/>
+      <c r="AB19" s="75"/>
+      <c r="AC19" s="75"/>
+      <c r="AD19" s="80"/>
     </row>
     <row r="20" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="59"/>
-      <c r="B20" s="60"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="42"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="42"/>
-      <c r="K20" s="42"/>
-      <c r="L20" s="42"/>
-      <c r="M20" s="42"/>
-      <c r="N20" s="42"/>
-      <c r="O20" s="42"/>
-      <c r="P20" s="42"/>
-      <c r="Q20" s="42"/>
-      <c r="R20" s="43"/>
+      <c r="A20" s="137"/>
+      <c r="B20" s="138"/>
+      <c r="C20" s="76"/>
+      <c r="D20" s="84"/>
+      <c r="E20" s="84"/>
+      <c r="F20" s="84"/>
+      <c r="G20" s="84"/>
+      <c r="H20" s="84"/>
+      <c r="I20" s="84"/>
+      <c r="J20" s="84"/>
+      <c r="K20" s="84"/>
+      <c r="L20" s="84"/>
+      <c r="M20" s="84"/>
+      <c r="N20" s="84"/>
+      <c r="O20" s="84"/>
+      <c r="P20" s="84"/>
+      <c r="Q20" s="84"/>
+      <c r="R20" s="74"/>
       <c r="S20" s="2"/>
       <c r="T20" s="2"/>
       <c r="U20" s="7"/>
       <c r="V20" s="2"/>
       <c r="W20" s="2"/>
       <c r="X20" s="2"/>
-      <c r="Y20" s="44"/>
-      <c r="Z20" s="44"/>
-      <c r="AA20" s="44"/>
-      <c r="AB20" s="44"/>
-      <c r="AC20" s="44"/>
-      <c r="AD20" s="45"/>
+      <c r="Y20" s="75"/>
+      <c r="Z20" s="75"/>
+      <c r="AA20" s="75"/>
+      <c r="AB20" s="75"/>
+      <c r="AC20" s="75"/>
+      <c r="AD20" s="80"/>
     </row>
     <row r="21" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="59"/>
-      <c r="B21" s="60"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="42"/>
-      <c r="K21" s="42"/>
-      <c r="L21" s="42"/>
-      <c r="M21" s="42"/>
-      <c r="N21" s="42"/>
-      <c r="O21" s="42"/>
-      <c r="P21" s="42"/>
-      <c r="Q21" s="42"/>
-      <c r="R21" s="43"/>
+      <c r="A21" s="137"/>
+      <c r="B21" s="138"/>
+      <c r="C21" s="76"/>
+      <c r="D21" s="84"/>
+      <c r="E21" s="84"/>
+      <c r="F21" s="84"/>
+      <c r="G21" s="84"/>
+      <c r="H21" s="84"/>
+      <c r="I21" s="84"/>
+      <c r="J21" s="84"/>
+      <c r="K21" s="84"/>
+      <c r="L21" s="84"/>
+      <c r="M21" s="84"/>
+      <c r="N21" s="84"/>
+      <c r="O21" s="84"/>
+      <c r="P21" s="84"/>
+      <c r="Q21" s="84"/>
+      <c r="R21" s="74"/>
       <c r="S21" s="2"/>
       <c r="T21" s="2"/>
       <c r="U21" s="7"/>
       <c r="V21" s="2"/>
       <c r="W21" s="2"/>
       <c r="X21" s="2"/>
-      <c r="Y21" s="44"/>
-      <c r="Z21" s="44"/>
-      <c r="AA21" s="44"/>
-      <c r="AB21" s="44"/>
-      <c r="AC21" s="44"/>
-      <c r="AD21" s="45"/>
+      <c r="Y21" s="75"/>
+      <c r="Z21" s="75"/>
+      <c r="AA21" s="75"/>
+      <c r="AB21" s="75"/>
+      <c r="AC21" s="75"/>
+      <c r="AD21" s="80"/>
     </row>
     <row r="22" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="59"/>
-      <c r="B22" s="60"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="42"/>
-      <c r="H22" s="42"/>
-      <c r="I22" s="42"/>
-      <c r="J22" s="42"/>
-      <c r="K22" s="42"/>
-      <c r="L22" s="42"/>
-      <c r="M22" s="42"/>
-      <c r="N22" s="42"/>
-      <c r="O22" s="42"/>
-      <c r="P22" s="42"/>
-      <c r="Q22" s="42"/>
-      <c r="R22" s="43"/>
+      <c r="A22" s="137"/>
+      <c r="B22" s="138"/>
+      <c r="C22" s="76"/>
+      <c r="D22" s="84"/>
+      <c r="E22" s="84"/>
+      <c r="F22" s="84"/>
+      <c r="G22" s="84"/>
+      <c r="H22" s="84"/>
+      <c r="I22" s="84"/>
+      <c r="J22" s="84"/>
+      <c r="K22" s="84"/>
+      <c r="L22" s="84"/>
+      <c r="M22" s="84"/>
+      <c r="N22" s="84"/>
+      <c r="O22" s="84"/>
+      <c r="P22" s="84"/>
+      <c r="Q22" s="84"/>
+      <c r="R22" s="74"/>
       <c r="S22" s="2"/>
       <c r="T22" s="2"/>
       <c r="U22" s="7"/>
       <c r="V22" s="2"/>
       <c r="W22" s="2"/>
       <c r="X22" s="2"/>
-      <c r="Y22" s="44"/>
-      <c r="Z22" s="44"/>
-      <c r="AA22" s="44"/>
-      <c r="AB22" s="44"/>
-      <c r="AC22" s="44"/>
-      <c r="AD22" s="45"/>
+      <c r="Y22" s="75"/>
+      <c r="Z22" s="75"/>
+      <c r="AA22" s="75"/>
+      <c r="AB22" s="75"/>
+      <c r="AC22" s="75"/>
+      <c r="AD22" s="80"/>
     </row>
     <row r="23" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="59"/>
-      <c r="B23" s="60"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="42"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="42"/>
-      <c r="I23" s="42"/>
-      <c r="J23" s="42"/>
-      <c r="K23" s="42"/>
-      <c r="L23" s="42"/>
-      <c r="M23" s="42"/>
-      <c r="N23" s="42"/>
-      <c r="O23" s="42"/>
-      <c r="P23" s="42"/>
-      <c r="Q23" s="42"/>
-      <c r="R23" s="43"/>
+      <c r="A23" s="137"/>
+      <c r="B23" s="138"/>
+      <c r="C23" s="76"/>
+      <c r="D23" s="84"/>
+      <c r="E23" s="84"/>
+      <c r="F23" s="84"/>
+      <c r="G23" s="84"/>
+      <c r="H23" s="84"/>
+      <c r="I23" s="84"/>
+      <c r="J23" s="84"/>
+      <c r="K23" s="84"/>
+      <c r="L23" s="84"/>
+      <c r="M23" s="84"/>
+      <c r="N23" s="84"/>
+      <c r="O23" s="84"/>
+      <c r="P23" s="84"/>
+      <c r="Q23" s="84"/>
+      <c r="R23" s="74"/>
       <c r="S23" s="2"/>
       <c r="T23" s="2"/>
       <c r="U23" s="7"/>
       <c r="V23" s="2"/>
       <c r="W23" s="2"/>
       <c r="X23" s="2"/>
-      <c r="Y23" s="44"/>
-      <c r="Z23" s="44"/>
-      <c r="AA23" s="44"/>
-      <c r="AB23" s="44"/>
-      <c r="AC23" s="44"/>
-      <c r="AD23" s="45"/>
+      <c r="Y23" s="75"/>
+      <c r="Z23" s="75"/>
+      <c r="AA23" s="75"/>
+      <c r="AB23" s="75"/>
+      <c r="AC23" s="75"/>
+      <c r="AD23" s="80"/>
     </row>
     <row r="24" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="59"/>
-      <c r="B24" s="60"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="42"/>
-      <c r="J24" s="42"/>
-      <c r="K24" s="42"/>
-      <c r="L24" s="42"/>
-      <c r="M24" s="42"/>
-      <c r="N24" s="42"/>
-      <c r="O24" s="42"/>
-      <c r="P24" s="42"/>
-      <c r="Q24" s="42"/>
-      <c r="R24" s="43"/>
+      <c r="A24" s="137"/>
+      <c r="B24" s="138"/>
+      <c r="C24" s="76"/>
+      <c r="D24" s="84"/>
+      <c r="E24" s="84"/>
+      <c r="F24" s="84"/>
+      <c r="G24" s="84"/>
+      <c r="H24" s="84"/>
+      <c r="I24" s="84"/>
+      <c r="J24" s="84"/>
+      <c r="K24" s="84"/>
+      <c r="L24" s="84"/>
+      <c r="M24" s="84"/>
+      <c r="N24" s="84"/>
+      <c r="O24" s="84"/>
+      <c r="P24" s="84"/>
+      <c r="Q24" s="84"/>
+      <c r="R24" s="74"/>
       <c r="S24" s="2"/>
       <c r="T24" s="2"/>
       <c r="U24" s="7"/>
       <c r="V24" s="2"/>
       <c r="W24" s="2"/>
       <c r="X24" s="2"/>
-      <c r="Y24" s="44"/>
-      <c r="Z24" s="44"/>
-      <c r="AA24" s="44"/>
-      <c r="AB24" s="44"/>
-      <c r="AC24" s="44"/>
-      <c r="AD24" s="45"/>
+      <c r="Y24" s="75"/>
+      <c r="Z24" s="75"/>
+      <c r="AA24" s="75"/>
+      <c r="AB24" s="75"/>
+      <c r="AC24" s="75"/>
+      <c r="AD24" s="80"/>
     </row>
     <row r="25" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="59"/>
-      <c r="B25" s="60"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
-      <c r="F25" s="42"/>
-      <c r="G25" s="42"/>
-      <c r="H25" s="42"/>
-      <c r="I25" s="42"/>
-      <c r="J25" s="42"/>
-      <c r="K25" s="42"/>
-      <c r="L25" s="42"/>
-      <c r="M25" s="42"/>
-      <c r="N25" s="42"/>
-      <c r="O25" s="42"/>
-      <c r="P25" s="42"/>
-      <c r="Q25" s="42"/>
-      <c r="R25" s="43"/>
+      <c r="A25" s="137"/>
+      <c r="B25" s="138"/>
+      <c r="C25" s="76"/>
+      <c r="D25" s="84"/>
+      <c r="E25" s="84"/>
+      <c r="F25" s="84"/>
+      <c r="G25" s="84"/>
+      <c r="H25" s="84"/>
+      <c r="I25" s="84"/>
+      <c r="J25" s="84"/>
+      <c r="K25" s="84"/>
+      <c r="L25" s="84"/>
+      <c r="M25" s="84"/>
+      <c r="N25" s="84"/>
+      <c r="O25" s="84"/>
+      <c r="P25" s="84"/>
+      <c r="Q25" s="84"/>
+      <c r="R25" s="74"/>
       <c r="S25" s="2"/>
       <c r="T25" s="2"/>
       <c r="U25" s="7"/>
       <c r="V25" s="2"/>
       <c r="W25" s="2"/>
       <c r="X25" s="2"/>
-      <c r="Y25" s="44"/>
-      <c r="Z25" s="44"/>
-      <c r="AA25" s="44"/>
-      <c r="AB25" s="44"/>
-      <c r="AC25" s="44"/>
-      <c r="AD25" s="45"/>
+      <c r="Y25" s="75"/>
+      <c r="Z25" s="75"/>
+      <c r="AA25" s="75"/>
+      <c r="AB25" s="75"/>
+      <c r="AC25" s="75"/>
+      <c r="AD25" s="80"/>
     </row>
     <row r="26" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="59"/>
-      <c r="B26" s="60"/>
-      <c r="C26" s="41"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="42"/>
-      <c r="J26" s="42"/>
-      <c r="K26" s="42"/>
-      <c r="L26" s="42"/>
-      <c r="M26" s="42"/>
-      <c r="N26" s="42"/>
-      <c r="O26" s="42"/>
-      <c r="P26" s="42"/>
-      <c r="Q26" s="42"/>
-      <c r="R26" s="43"/>
+      <c r="A26" s="137"/>
+      <c r="B26" s="138"/>
+      <c r="C26" s="76"/>
+      <c r="D26" s="84"/>
+      <c r="E26" s="84"/>
+      <c r="F26" s="84"/>
+      <c r="G26" s="84"/>
+      <c r="H26" s="84"/>
+      <c r="I26" s="84"/>
+      <c r="J26" s="84"/>
+      <c r="K26" s="84"/>
+      <c r="L26" s="84"/>
+      <c r="M26" s="84"/>
+      <c r="N26" s="84"/>
+      <c r="O26" s="84"/>
+      <c r="P26" s="84"/>
+      <c r="Q26" s="84"/>
+      <c r="R26" s="74"/>
       <c r="S26" s="2"/>
       <c r="T26" s="2"/>
       <c r="U26" s="7"/>
       <c r="V26" s="2"/>
       <c r="W26" s="2"/>
       <c r="X26" s="2"/>
-      <c r="Y26" s="44"/>
-      <c r="Z26" s="44"/>
-      <c r="AA26" s="44"/>
-      <c r="AB26" s="44"/>
-      <c r="AC26" s="44"/>
-      <c r="AD26" s="45"/>
+      <c r="Y26" s="75"/>
+      <c r="Z26" s="75"/>
+      <c r="AA26" s="75"/>
+      <c r="AB26" s="75"/>
+      <c r="AC26" s="75"/>
+      <c r="AD26" s="80"/>
     </row>
     <row r="27" spans="1:30" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="61"/>
-      <c r="B27" s="62"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="51"/>
-      <c r="E27" s="51"/>
-      <c r="F27" s="51"/>
-      <c r="G27" s="51"/>
-      <c r="H27" s="51"/>
-      <c r="I27" s="51"/>
-      <c r="J27" s="51"/>
-      <c r="K27" s="51"/>
-      <c r="L27" s="51"/>
-      <c r="M27" s="51"/>
-      <c r="N27" s="51"/>
-      <c r="O27" s="51"/>
-      <c r="P27" s="51"/>
-      <c r="Q27" s="51"/>
+      <c r="A27" s="139"/>
+      <c r="B27" s="140"/>
+      <c r="C27" s="48"/>
+      <c r="D27" s="146"/>
+      <c r="E27" s="146"/>
+      <c r="F27" s="146"/>
+      <c r="G27" s="146"/>
+      <c r="H27" s="146"/>
+      <c r="I27" s="146"/>
+      <c r="J27" s="146"/>
+      <c r="K27" s="146"/>
+      <c r="L27" s="146"/>
+      <c r="M27" s="146"/>
+      <c r="N27" s="146"/>
+      <c r="O27" s="146"/>
+      <c r="P27" s="146"/>
+      <c r="Q27" s="146"/>
       <c r="R27" s="46"/>
       <c r="S27" s="4"/>
       <c r="T27" s="4"/>
@@ -3617,526 +3620,526 @@
       <c r="V27" s="2"/>
       <c r="W27" s="2"/>
       <c r="X27" s="4"/>
-      <c r="Y27" s="44"/>
-      <c r="Z27" s="44"/>
-      <c r="AA27" s="44"/>
-      <c r="AB27" s="44"/>
-      <c r="AC27" s="44"/>
-      <c r="AD27" s="45"/>
+      <c r="Y27" s="75"/>
+      <c r="Z27" s="75"/>
+      <c r="AA27" s="75"/>
+      <c r="AB27" s="75"/>
+      <c r="AC27" s="75"/>
+      <c r="AD27" s="80"/>
     </row>
     <row r="28" spans="1:30" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="57" t="s">
+      <c r="A28" s="143" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="58"/>
-      <c r="C28" s="55" t="s">
+      <c r="B28" s="144"/>
+      <c r="C28" s="121" t="s">
         <v>3</v>
       </c>
-      <c r="D28" s="63"/>
-      <c r="E28" s="63"/>
-      <c r="F28" s="63" t="s">
+      <c r="D28" s="145"/>
+      <c r="E28" s="145"/>
+      <c r="F28" s="145" t="s">
         <v>1</v>
       </c>
-      <c r="G28" s="63"/>
-      <c r="H28" s="63"/>
-      <c r="I28" s="63" t="s">
+      <c r="G28" s="145"/>
+      <c r="H28" s="145"/>
+      <c r="I28" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="J28" s="63"/>
-      <c r="K28" s="63"/>
-      <c r="L28" s="63"/>
-      <c r="M28" s="63" t="s">
+      <c r="J28" s="145"/>
+      <c r="K28" s="145"/>
+      <c r="L28" s="145"/>
+      <c r="M28" s="145" t="s">
         <v>5</v>
       </c>
-      <c r="N28" s="63"/>
-      <c r="O28" s="63"/>
-      <c r="P28" s="63"/>
-      <c r="Q28" s="63"/>
-      <c r="R28" s="63"/>
-      <c r="S28" s="63" t="s">
+      <c r="N28" s="145"/>
+      <c r="O28" s="145"/>
+      <c r="P28" s="145"/>
+      <c r="Q28" s="145"/>
+      <c r="R28" s="145"/>
+      <c r="S28" s="145" t="s">
         <v>6</v>
       </c>
-      <c r="T28" s="63"/>
-      <c r="U28" s="63"/>
-      <c r="V28" s="63"/>
-      <c r="W28" s="63"/>
-      <c r="X28" s="63"/>
-      <c r="Y28" s="63"/>
-      <c r="Z28" s="63"/>
-      <c r="AA28" s="63" t="s">
+      <c r="T28" s="145"/>
+      <c r="U28" s="145"/>
+      <c r="V28" s="145"/>
+      <c r="W28" s="145"/>
+      <c r="X28" s="145"/>
+      <c r="Y28" s="145"/>
+      <c r="Z28" s="145"/>
+      <c r="AA28" s="145" t="s">
         <v>7</v>
       </c>
-      <c r="AB28" s="63"/>
-      <c r="AC28" s="63"/>
-      <c r="AD28" s="64"/>
+      <c r="AB28" s="145"/>
+      <c r="AC28" s="145"/>
+      <c r="AD28" s="147"/>
     </row>
     <row r="29" spans="1:30" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="61"/>
-      <c r="B29" s="62"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="51"/>
-      <c r="H29" s="51"/>
-      <c r="I29" s="51"/>
-      <c r="J29" s="51"/>
-      <c r="K29" s="51"/>
-      <c r="L29" s="51"/>
-      <c r="M29" s="51"/>
-      <c r="N29" s="51"/>
-      <c r="O29" s="51"/>
-      <c r="P29" s="51"/>
-      <c r="Q29" s="51"/>
-      <c r="R29" s="51"/>
-      <c r="S29" s="51" t="s">
+      <c r="A29" s="139"/>
+      <c r="B29" s="140"/>
+      <c r="C29" s="48"/>
+      <c r="D29" s="146"/>
+      <c r="E29" s="146"/>
+      <c r="F29" s="146"/>
+      <c r="G29" s="146"/>
+      <c r="H29" s="146"/>
+      <c r="I29" s="146"/>
+      <c r="J29" s="146"/>
+      <c r="K29" s="146"/>
+      <c r="L29" s="146"/>
+      <c r="M29" s="146"/>
+      <c r="N29" s="146"/>
+      <c r="O29" s="146"/>
+      <c r="P29" s="146"/>
+      <c r="Q29" s="146"/>
+      <c r="R29" s="146"/>
+      <c r="S29" s="146" t="s">
         <v>8</v>
       </c>
-      <c r="T29" s="51"/>
-      <c r="U29" s="51"/>
-      <c r="V29" s="51"/>
-      <c r="W29" s="51"/>
-      <c r="X29" s="51"/>
-      <c r="Y29" s="51"/>
-      <c r="Z29" s="51"/>
-      <c r="AA29" s="51"/>
-      <c r="AB29" s="51"/>
-      <c r="AC29" s="51"/>
-      <c r="AD29" s="52"/>
+      <c r="T29" s="146"/>
+      <c r="U29" s="146"/>
+      <c r="V29" s="146"/>
+      <c r="W29" s="146"/>
+      <c r="X29" s="146"/>
+      <c r="Y29" s="146"/>
+      <c r="Z29" s="146"/>
+      <c r="AA29" s="146"/>
+      <c r="AB29" s="146"/>
+      <c r="AC29" s="146"/>
+      <c r="AD29" s="148"/>
     </row>
     <row r="30" spans="1:30" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="57" t="s">
-        <v>47</v>
-      </c>
-      <c r="B30" s="58"/>
-      <c r="C30" s="55" t="s">
+      <c r="A30" s="143" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="144"/>
+      <c r="C30" s="121" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" s="145"/>
+      <c r="E30" s="145"/>
+      <c r="F30" s="145"/>
+      <c r="G30" s="145"/>
+      <c r="H30" s="119" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="63"/>
-      <c r="E30" s="63"/>
-      <c r="F30" s="63"/>
-      <c r="G30" s="63"/>
-      <c r="H30" s="53" t="s">
+      <c r="I30" s="120"/>
+      <c r="J30" s="120"/>
+      <c r="K30" s="120"/>
+      <c r="L30" s="120"/>
+      <c r="M30" s="121"/>
+      <c r="N30" s="119" t="s">
         <v>39</v>
       </c>
-      <c r="I30" s="54"/>
-      <c r="J30" s="54"/>
-      <c r="K30" s="54"/>
-      <c r="L30" s="54"/>
-      <c r="M30" s="55"/>
-      <c r="N30" s="53" t="s">
+      <c r="O30" s="120"/>
+      <c r="P30" s="120"/>
+      <c r="Q30" s="120"/>
+      <c r="R30" s="120"/>
+      <c r="S30" s="120"/>
+      <c r="T30" s="121"/>
+      <c r="U30" s="119" t="s">
         <v>40</v>
       </c>
-      <c r="O30" s="54"/>
-      <c r="P30" s="54"/>
-      <c r="Q30" s="54"/>
-      <c r="R30" s="54"/>
-      <c r="S30" s="54"/>
-      <c r="T30" s="55"/>
-      <c r="U30" s="53" t="s">
+      <c r="V30" s="120"/>
+      <c r="W30" s="120"/>
+      <c r="X30" s="121"/>
+      <c r="Y30" s="119" t="s">
         <v>41</v>
       </c>
-      <c r="V30" s="54"/>
-      <c r="W30" s="54"/>
-      <c r="X30" s="55"/>
-      <c r="Y30" s="53" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z30" s="54"/>
-      <c r="AA30" s="54"/>
-      <c r="AB30" s="54"/>
-      <c r="AC30" s="54"/>
-      <c r="AD30" s="56"/>
+      <c r="Z30" s="120"/>
+      <c r="AA30" s="120"/>
+      <c r="AB30" s="120"/>
+      <c r="AC30" s="120"/>
+      <c r="AD30" s="122"/>
     </row>
     <row r="31" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="59"/>
-      <c r="B31" s="60"/>
-      <c r="C31" s="41" t="s">
-        <v>92</v>
-      </c>
-      <c r="D31" s="42"/>
-      <c r="E31" s="42"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="42"/>
-      <c r="H31" s="43" t="s">
+      <c r="A31" s="137"/>
+      <c r="B31" s="138"/>
+      <c r="C31" s="76" t="s">
+        <v>91</v>
+      </c>
+      <c r="D31" s="84"/>
+      <c r="E31" s="84"/>
+      <c r="F31" s="84"/>
+      <c r="G31" s="84"/>
+      <c r="H31" s="74" t="s">
+        <v>88</v>
+      </c>
+      <c r="I31" s="75"/>
+      <c r="J31" s="75"/>
+      <c r="K31" s="75"/>
+      <c r="L31" s="75"/>
+      <c r="M31" s="76"/>
+      <c r="N31" s="74" t="s">
         <v>89</v>
       </c>
-      <c r="I31" s="44"/>
-      <c r="J31" s="44"/>
-      <c r="K31" s="44"/>
-      <c r="L31" s="44"/>
-      <c r="M31" s="41"/>
-      <c r="N31" s="43" t="s">
+      <c r="O31" s="75"/>
+      <c r="P31" s="75"/>
+      <c r="Q31" s="75"/>
+      <c r="R31" s="75"/>
+      <c r="S31" s="75"/>
+      <c r="T31" s="76"/>
+      <c r="U31" s="74" t="s">
         <v>90</v>
       </c>
-      <c r="O31" s="44"/>
-      <c r="P31" s="44"/>
-      <c r="Q31" s="44"/>
-      <c r="R31" s="44"/>
-      <c r="S31" s="44"/>
-      <c r="T31" s="41"/>
-      <c r="U31" s="43" t="s">
-        <v>91</v>
-      </c>
-      <c r="V31" s="44"/>
-      <c r="W31" s="44"/>
-      <c r="X31" s="41"/>
-      <c r="Y31" s="43" t="s">
-        <v>89</v>
-      </c>
-      <c r="Z31" s="44"/>
-      <c r="AA31" s="44"/>
-      <c r="AB31" s="44"/>
-      <c r="AC31" s="44"/>
-      <c r="AD31" s="45"/>
+      <c r="V31" s="75"/>
+      <c r="W31" s="75"/>
+      <c r="X31" s="76"/>
+      <c r="Y31" s="74" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z31" s="75"/>
+      <c r="AA31" s="75"/>
+      <c r="AB31" s="75"/>
+      <c r="AC31" s="75"/>
+      <c r="AD31" s="80"/>
     </row>
     <row r="32" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="59"/>
-      <c r="B32" s="60"/>
-      <c r="C32" s="41" t="s">
+      <c r="A32" s="137"/>
+      <c r="B32" s="138"/>
+      <c r="C32" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="D32" s="42"/>
-      <c r="E32" s="42"/>
-      <c r="F32" s="42"/>
-      <c r="G32" s="42"/>
-      <c r="H32" s="43"/>
-      <c r="I32" s="44"/>
-      <c r="J32" s="44"/>
-      <c r="K32" s="44"/>
-      <c r="L32" s="44"/>
-      <c r="M32" s="41"/>
-      <c r="N32" s="43"/>
-      <c r="O32" s="44"/>
-      <c r="P32" s="44"/>
-      <c r="Q32" s="44"/>
-      <c r="R32" s="44"/>
-      <c r="S32" s="44"/>
-      <c r="T32" s="41"/>
-      <c r="U32" s="43"/>
-      <c r="V32" s="44"/>
-      <c r="W32" s="44"/>
-      <c r="X32" s="41"/>
-      <c r="Y32" s="43"/>
-      <c r="Z32" s="44"/>
-      <c r="AA32" s="44"/>
-      <c r="AB32" s="44"/>
-      <c r="AC32" s="44"/>
-      <c r="AD32" s="45"/>
+      <c r="D32" s="84"/>
+      <c r="E32" s="84"/>
+      <c r="F32" s="84"/>
+      <c r="G32" s="84"/>
+      <c r="H32" s="74"/>
+      <c r="I32" s="75"/>
+      <c r="J32" s="75"/>
+      <c r="K32" s="75"/>
+      <c r="L32" s="75"/>
+      <c r="M32" s="76"/>
+      <c r="N32" s="74"/>
+      <c r="O32" s="75"/>
+      <c r="P32" s="75"/>
+      <c r="Q32" s="75"/>
+      <c r="R32" s="75"/>
+      <c r="S32" s="75"/>
+      <c r="T32" s="76"/>
+      <c r="U32" s="74"/>
+      <c r="V32" s="75"/>
+      <c r="W32" s="75"/>
+      <c r="X32" s="76"/>
+      <c r="Y32" s="74"/>
+      <c r="Z32" s="75"/>
+      <c r="AA32" s="75"/>
+      <c r="AB32" s="75"/>
+      <c r="AC32" s="75"/>
+      <c r="AD32" s="80"/>
     </row>
     <row r="33" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="59"/>
-      <c r="B33" s="60"/>
-      <c r="C33" s="41" t="s">
+      <c r="A33" s="137"/>
+      <c r="B33" s="138"/>
+      <c r="C33" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="D33" s="42"/>
-      <c r="E33" s="42"/>
-      <c r="F33" s="42"/>
-      <c r="G33" s="42"/>
-      <c r="H33" s="43"/>
-      <c r="I33" s="44"/>
-      <c r="J33" s="44"/>
-      <c r="K33" s="44"/>
-      <c r="L33" s="44"/>
-      <c r="M33" s="41"/>
-      <c r="N33" s="43"/>
-      <c r="O33" s="44"/>
-      <c r="P33" s="44"/>
-      <c r="Q33" s="44"/>
-      <c r="R33" s="44"/>
-      <c r="S33" s="44"/>
-      <c r="T33" s="41"/>
-      <c r="U33" s="43"/>
-      <c r="V33" s="44"/>
-      <c r="W33" s="44"/>
-      <c r="X33" s="41"/>
-      <c r="Y33" s="43"/>
-      <c r="Z33" s="44"/>
-      <c r="AA33" s="44"/>
-      <c r="AB33" s="44"/>
-      <c r="AC33" s="44"/>
-      <c r="AD33" s="45"/>
+      <c r="D33" s="84"/>
+      <c r="E33" s="84"/>
+      <c r="F33" s="84"/>
+      <c r="G33" s="84"/>
+      <c r="H33" s="74"/>
+      <c r="I33" s="75"/>
+      <c r="J33" s="75"/>
+      <c r="K33" s="75"/>
+      <c r="L33" s="75"/>
+      <c r="M33" s="76"/>
+      <c r="N33" s="74"/>
+      <c r="O33" s="75"/>
+      <c r="P33" s="75"/>
+      <c r="Q33" s="75"/>
+      <c r="R33" s="75"/>
+      <c r="S33" s="75"/>
+      <c r="T33" s="76"/>
+      <c r="U33" s="74"/>
+      <c r="V33" s="75"/>
+      <c r="W33" s="75"/>
+      <c r="X33" s="76"/>
+      <c r="Y33" s="74"/>
+      <c r="Z33" s="75"/>
+      <c r="AA33" s="75"/>
+      <c r="AB33" s="75"/>
+      <c r="AC33" s="75"/>
+      <c r="AD33" s="80"/>
     </row>
     <row r="34" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="59"/>
-      <c r="B34" s="60"/>
-      <c r="C34" s="41" t="s">
+      <c r="A34" s="137"/>
+      <c r="B34" s="138"/>
+      <c r="C34" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="D34" s="42"/>
-      <c r="E34" s="42"/>
-      <c r="F34" s="42"/>
-      <c r="G34" s="42"/>
-      <c r="H34" s="43"/>
-      <c r="I34" s="44"/>
-      <c r="J34" s="44"/>
-      <c r="K34" s="44"/>
-      <c r="L34" s="44"/>
-      <c r="M34" s="41"/>
-      <c r="N34" s="43"/>
-      <c r="O34" s="44"/>
-      <c r="P34" s="44"/>
-      <c r="Q34" s="44"/>
-      <c r="R34" s="44"/>
-      <c r="S34" s="44"/>
-      <c r="T34" s="41"/>
-      <c r="U34" s="43"/>
-      <c r="V34" s="44"/>
-      <c r="W34" s="44"/>
-      <c r="X34" s="41"/>
-      <c r="Y34" s="43"/>
-      <c r="Z34" s="44"/>
-      <c r="AA34" s="44"/>
-      <c r="AB34" s="44"/>
-      <c r="AC34" s="44"/>
-      <c r="AD34" s="45"/>
+      <c r="D34" s="84"/>
+      <c r="E34" s="84"/>
+      <c r="F34" s="84"/>
+      <c r="G34" s="84"/>
+      <c r="H34" s="74"/>
+      <c r="I34" s="75"/>
+      <c r="J34" s="75"/>
+      <c r="K34" s="75"/>
+      <c r="L34" s="75"/>
+      <c r="M34" s="76"/>
+      <c r="N34" s="74"/>
+      <c r="O34" s="75"/>
+      <c r="P34" s="75"/>
+      <c r="Q34" s="75"/>
+      <c r="R34" s="75"/>
+      <c r="S34" s="75"/>
+      <c r="T34" s="76"/>
+      <c r="U34" s="74"/>
+      <c r="V34" s="75"/>
+      <c r="W34" s="75"/>
+      <c r="X34" s="76"/>
+      <c r="Y34" s="74"/>
+      <c r="Z34" s="75"/>
+      <c r="AA34" s="75"/>
+      <c r="AB34" s="75"/>
+      <c r="AC34" s="75"/>
+      <c r="AD34" s="80"/>
     </row>
     <row r="35" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="59"/>
-      <c r="B35" s="60"/>
-      <c r="C35" s="41" t="s">
+      <c r="A35" s="137"/>
+      <c r="B35" s="138"/>
+      <c r="C35" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="D35" s="42"/>
-      <c r="E35" s="42"/>
-      <c r="F35" s="42"/>
-      <c r="G35" s="42"/>
-      <c r="H35" s="43"/>
-      <c r="I35" s="44"/>
-      <c r="J35" s="44"/>
-      <c r="K35" s="44"/>
-      <c r="L35" s="44"/>
-      <c r="M35" s="41"/>
-      <c r="N35" s="43"/>
-      <c r="O35" s="44"/>
-      <c r="P35" s="44"/>
-      <c r="Q35" s="44"/>
-      <c r="R35" s="44"/>
-      <c r="S35" s="44"/>
-      <c r="T35" s="41"/>
-      <c r="U35" s="43"/>
-      <c r="V35" s="44"/>
-      <c r="W35" s="44"/>
-      <c r="X35" s="41"/>
-      <c r="Y35" s="43"/>
-      <c r="Z35" s="44"/>
-      <c r="AA35" s="44"/>
-      <c r="AB35" s="44"/>
-      <c r="AC35" s="44"/>
-      <c r="AD35" s="45"/>
+      <c r="D35" s="84"/>
+      <c r="E35" s="84"/>
+      <c r="F35" s="84"/>
+      <c r="G35" s="84"/>
+      <c r="H35" s="74"/>
+      <c r="I35" s="75"/>
+      <c r="J35" s="75"/>
+      <c r="K35" s="75"/>
+      <c r="L35" s="75"/>
+      <c r="M35" s="76"/>
+      <c r="N35" s="74"/>
+      <c r="O35" s="75"/>
+      <c r="P35" s="75"/>
+      <c r="Q35" s="75"/>
+      <c r="R35" s="75"/>
+      <c r="S35" s="75"/>
+      <c r="T35" s="76"/>
+      <c r="U35" s="74"/>
+      <c r="V35" s="75"/>
+      <c r="W35" s="75"/>
+      <c r="X35" s="76"/>
+      <c r="Y35" s="74"/>
+      <c r="Z35" s="75"/>
+      <c r="AA35" s="75"/>
+      <c r="AB35" s="75"/>
+      <c r="AC35" s="75"/>
+      <c r="AD35" s="80"/>
     </row>
     <row r="36" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="59"/>
-      <c r="B36" s="60"/>
-      <c r="C36" s="41" t="s">
+      <c r="A36" s="137"/>
+      <c r="B36" s="138"/>
+      <c r="C36" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="D36" s="42"/>
-      <c r="E36" s="42"/>
-      <c r="F36" s="42"/>
-      <c r="G36" s="42"/>
-      <c r="H36" s="43"/>
-      <c r="I36" s="44"/>
-      <c r="J36" s="44"/>
-      <c r="K36" s="44"/>
-      <c r="L36" s="44"/>
-      <c r="M36" s="41"/>
-      <c r="N36" s="43"/>
-      <c r="O36" s="44"/>
-      <c r="P36" s="44"/>
-      <c r="Q36" s="44"/>
-      <c r="R36" s="44"/>
-      <c r="S36" s="44"/>
-      <c r="T36" s="41"/>
-      <c r="U36" s="43"/>
-      <c r="V36" s="44"/>
-      <c r="W36" s="44"/>
-      <c r="X36" s="41"/>
-      <c r="Y36" s="43"/>
-      <c r="Z36" s="44"/>
-      <c r="AA36" s="44"/>
-      <c r="AB36" s="44"/>
-      <c r="AC36" s="44"/>
-      <c r="AD36" s="45"/>
+      <c r="D36" s="84"/>
+      <c r="E36" s="84"/>
+      <c r="F36" s="84"/>
+      <c r="G36" s="84"/>
+      <c r="H36" s="74"/>
+      <c r="I36" s="75"/>
+      <c r="J36" s="75"/>
+      <c r="K36" s="75"/>
+      <c r="L36" s="75"/>
+      <c r="M36" s="76"/>
+      <c r="N36" s="74"/>
+      <c r="O36" s="75"/>
+      <c r="P36" s="75"/>
+      <c r="Q36" s="75"/>
+      <c r="R36" s="75"/>
+      <c r="S36" s="75"/>
+      <c r="T36" s="76"/>
+      <c r="U36" s="74"/>
+      <c r="V36" s="75"/>
+      <c r="W36" s="75"/>
+      <c r="X36" s="76"/>
+      <c r="Y36" s="74"/>
+      <c r="Z36" s="75"/>
+      <c r="AA36" s="75"/>
+      <c r="AB36" s="75"/>
+      <c r="AC36" s="75"/>
+      <c r="AD36" s="80"/>
     </row>
     <row r="37" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="59"/>
-      <c r="B37" s="60"/>
-      <c r="C37" s="41" t="s">
+      <c r="A37" s="137"/>
+      <c r="B37" s="138"/>
+      <c r="C37" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="D37" s="42"/>
-      <c r="E37" s="42"/>
-      <c r="F37" s="42"/>
-      <c r="G37" s="42"/>
-      <c r="H37" s="43"/>
-      <c r="I37" s="44"/>
-      <c r="J37" s="44"/>
-      <c r="K37" s="44"/>
-      <c r="L37" s="44"/>
-      <c r="M37" s="41"/>
-      <c r="N37" s="43"/>
-      <c r="O37" s="44"/>
-      <c r="P37" s="44"/>
-      <c r="Q37" s="44"/>
-      <c r="R37" s="44"/>
-      <c r="S37" s="44"/>
-      <c r="T37" s="41"/>
-      <c r="U37" s="43"/>
-      <c r="V37" s="44"/>
-      <c r="W37" s="44"/>
-      <c r="X37" s="41"/>
-      <c r="Y37" s="43"/>
-      <c r="Z37" s="44"/>
-      <c r="AA37" s="44"/>
-      <c r="AB37" s="44"/>
-      <c r="AC37" s="44"/>
-      <c r="AD37" s="45"/>
+      <c r="D37" s="84"/>
+      <c r="E37" s="84"/>
+      <c r="F37" s="84"/>
+      <c r="G37" s="84"/>
+      <c r="H37" s="74"/>
+      <c r="I37" s="75"/>
+      <c r="J37" s="75"/>
+      <c r="K37" s="75"/>
+      <c r="L37" s="75"/>
+      <c r="M37" s="76"/>
+      <c r="N37" s="74"/>
+      <c r="O37" s="75"/>
+      <c r="P37" s="75"/>
+      <c r="Q37" s="75"/>
+      <c r="R37" s="75"/>
+      <c r="S37" s="75"/>
+      <c r="T37" s="76"/>
+      <c r="U37" s="74"/>
+      <c r="V37" s="75"/>
+      <c r="W37" s="75"/>
+      <c r="X37" s="76"/>
+      <c r="Y37" s="74"/>
+      <c r="Z37" s="75"/>
+      <c r="AA37" s="75"/>
+      <c r="AB37" s="75"/>
+      <c r="AC37" s="75"/>
+      <c r="AD37" s="80"/>
     </row>
     <row r="38" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="59"/>
-      <c r="B38" s="60"/>
-      <c r="C38" s="41" t="s">
+      <c r="A38" s="137"/>
+      <c r="B38" s="138"/>
+      <c r="C38" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="D38" s="42"/>
-      <c r="E38" s="42"/>
-      <c r="F38" s="42"/>
-      <c r="G38" s="42"/>
-      <c r="H38" s="43"/>
-      <c r="I38" s="44"/>
-      <c r="J38" s="44"/>
-      <c r="K38" s="44"/>
-      <c r="L38" s="44"/>
-      <c r="M38" s="41"/>
-      <c r="N38" s="43"/>
-      <c r="O38" s="44"/>
-      <c r="P38" s="44"/>
-      <c r="Q38" s="44"/>
-      <c r="R38" s="44"/>
-      <c r="S38" s="44"/>
-      <c r="T38" s="41"/>
-      <c r="U38" s="43"/>
-      <c r="V38" s="44"/>
-      <c r="W38" s="44"/>
-      <c r="X38" s="41"/>
-      <c r="Y38" s="43"/>
-      <c r="Z38" s="44"/>
-      <c r="AA38" s="44"/>
-      <c r="AB38" s="44"/>
-      <c r="AC38" s="44"/>
-      <c r="AD38" s="45"/>
+      <c r="D38" s="84"/>
+      <c r="E38" s="84"/>
+      <c r="F38" s="84"/>
+      <c r="G38" s="84"/>
+      <c r="H38" s="74"/>
+      <c r="I38" s="75"/>
+      <c r="J38" s="75"/>
+      <c r="K38" s="75"/>
+      <c r="L38" s="75"/>
+      <c r="M38" s="76"/>
+      <c r="N38" s="74"/>
+      <c r="O38" s="75"/>
+      <c r="P38" s="75"/>
+      <c r="Q38" s="75"/>
+      <c r="R38" s="75"/>
+      <c r="S38" s="75"/>
+      <c r="T38" s="76"/>
+      <c r="U38" s="74"/>
+      <c r="V38" s="75"/>
+      <c r="W38" s="75"/>
+      <c r="X38" s="76"/>
+      <c r="Y38" s="74"/>
+      <c r="Z38" s="75"/>
+      <c r="AA38" s="75"/>
+      <c r="AB38" s="75"/>
+      <c r="AC38" s="75"/>
+      <c r="AD38" s="80"/>
     </row>
     <row r="39" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="59"/>
-      <c r="B39" s="60"/>
-      <c r="C39" s="41" t="s">
+      <c r="A39" s="137"/>
+      <c r="B39" s="138"/>
+      <c r="C39" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="D39" s="42"/>
-      <c r="E39" s="42"/>
-      <c r="F39" s="42"/>
-      <c r="G39" s="42"/>
-      <c r="H39" s="43"/>
-      <c r="I39" s="44"/>
-      <c r="J39" s="44"/>
-      <c r="K39" s="44"/>
-      <c r="L39" s="44"/>
-      <c r="M39" s="41"/>
-      <c r="N39" s="43"/>
-      <c r="O39" s="44"/>
-      <c r="P39" s="44"/>
-      <c r="Q39" s="44"/>
-      <c r="R39" s="44"/>
-      <c r="S39" s="44"/>
-      <c r="T39" s="41"/>
-      <c r="U39" s="43"/>
-      <c r="V39" s="44"/>
-      <c r="W39" s="44"/>
-      <c r="X39" s="41"/>
-      <c r="Y39" s="43"/>
-      <c r="Z39" s="44"/>
-      <c r="AA39" s="44"/>
-      <c r="AB39" s="44"/>
-      <c r="AC39" s="44"/>
-      <c r="AD39" s="45"/>
+      <c r="D39" s="84"/>
+      <c r="E39" s="84"/>
+      <c r="F39" s="84"/>
+      <c r="G39" s="84"/>
+      <c r="H39" s="74"/>
+      <c r="I39" s="75"/>
+      <c r="J39" s="75"/>
+      <c r="K39" s="75"/>
+      <c r="L39" s="75"/>
+      <c r="M39" s="76"/>
+      <c r="N39" s="74"/>
+      <c r="O39" s="75"/>
+      <c r="P39" s="75"/>
+      <c r="Q39" s="75"/>
+      <c r="R39" s="75"/>
+      <c r="S39" s="75"/>
+      <c r="T39" s="76"/>
+      <c r="U39" s="74"/>
+      <c r="V39" s="75"/>
+      <c r="W39" s="75"/>
+      <c r="X39" s="76"/>
+      <c r="Y39" s="74"/>
+      <c r="Z39" s="75"/>
+      <c r="AA39" s="75"/>
+      <c r="AB39" s="75"/>
+      <c r="AC39" s="75"/>
+      <c r="AD39" s="80"/>
     </row>
     <row r="40" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="59"/>
-      <c r="B40" s="60"/>
-      <c r="C40" s="41" t="s">
+      <c r="A40" s="137"/>
+      <c r="B40" s="138"/>
+      <c r="C40" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="D40" s="42"/>
-      <c r="E40" s="42"/>
-      <c r="F40" s="42"/>
-      <c r="G40" s="42"/>
-      <c r="H40" s="43"/>
-      <c r="I40" s="44"/>
-      <c r="J40" s="44"/>
-      <c r="K40" s="44"/>
-      <c r="L40" s="44"/>
-      <c r="M40" s="41"/>
-      <c r="N40" s="43"/>
-      <c r="O40" s="44"/>
-      <c r="P40" s="44"/>
-      <c r="Q40" s="44"/>
-      <c r="R40" s="44"/>
-      <c r="S40" s="44"/>
-      <c r="T40" s="41"/>
-      <c r="U40" s="43"/>
-      <c r="V40" s="44"/>
-      <c r="W40" s="44"/>
-      <c r="X40" s="41"/>
-      <c r="Y40" s="43"/>
-      <c r="Z40" s="44"/>
-      <c r="AA40" s="44"/>
-      <c r="AB40" s="44"/>
-      <c r="AC40" s="44"/>
-      <c r="AD40" s="45"/>
+      <c r="D40" s="84"/>
+      <c r="E40" s="84"/>
+      <c r="F40" s="84"/>
+      <c r="G40" s="84"/>
+      <c r="H40" s="74"/>
+      <c r="I40" s="75"/>
+      <c r="J40" s="75"/>
+      <c r="K40" s="75"/>
+      <c r="L40" s="75"/>
+      <c r="M40" s="76"/>
+      <c r="N40" s="74"/>
+      <c r="O40" s="75"/>
+      <c r="P40" s="75"/>
+      <c r="Q40" s="75"/>
+      <c r="R40" s="75"/>
+      <c r="S40" s="75"/>
+      <c r="T40" s="76"/>
+      <c r="U40" s="74"/>
+      <c r="V40" s="75"/>
+      <c r="W40" s="75"/>
+      <c r="X40" s="76"/>
+      <c r="Y40" s="74"/>
+      <c r="Z40" s="75"/>
+      <c r="AA40" s="75"/>
+      <c r="AB40" s="75"/>
+      <c r="AC40" s="75"/>
+      <c r="AD40" s="80"/>
     </row>
     <row r="41" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="59"/>
-      <c r="B41" s="60"/>
-      <c r="C41" s="49" t="s">
+      <c r="A41" s="137"/>
+      <c r="B41" s="138"/>
+      <c r="C41" s="149" t="s">
         <v>9</v>
       </c>
       <c r="D41" s="47"/>
       <c r="E41" s="47"/>
       <c r="F41" s="47"/>
-      <c r="G41" s="50"/>
+      <c r="G41" s="48"/>
       <c r="H41" s="46"/>
       <c r="I41" s="47"/>
       <c r="J41" s="47"/>
       <c r="K41" s="47"/>
       <c r="L41" s="47"/>
-      <c r="M41" s="50"/>
+      <c r="M41" s="48"/>
       <c r="N41" s="46"/>
       <c r="O41" s="47"/>
       <c r="P41" s="47"/>
       <c r="Q41" s="47"/>
       <c r="R41" s="47"/>
       <c r="S41" s="47"/>
-      <c r="T41" s="50"/>
+      <c r="T41" s="48"/>
       <c r="U41" s="46"/>
       <c r="V41" s="47"/>
       <c r="W41" s="47"/>
-      <c r="X41" s="50"/>
+      <c r="X41" s="48"/>
       <c r="Y41" s="46"/>
       <c r="Z41" s="47"/>
       <c r="AA41" s="47"/>
       <c r="AB41" s="47"/>
       <c r="AC41" s="47"/>
-      <c r="AD41" s="48"/>
+      <c r="AD41" s="83"/>
     </row>
     <row r="42" spans="1:30" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="59"/>
-      <c r="B42" s="60"/>
+      <c r="A42" s="137"/>
+      <c r="B42" s="138"/>
     </row>
     <row r="43" spans="1:30" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="61"/>
-      <c r="B43" s="62"/>
+      <c r="A43" s="139"/>
+      <c r="B43" s="140"/>
     </row>
     <row r="54" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C54" s="11"/>
@@ -9805,6 +9808,180 @@
     </row>
   </sheetData>
   <mergeCells count="198">
+    <mergeCell ref="C39:G39"/>
+    <mergeCell ref="H39:M39"/>
+    <mergeCell ref="N39:T39"/>
+    <mergeCell ref="U39:X39"/>
+    <mergeCell ref="Y39:AD39"/>
+    <mergeCell ref="C38:G38"/>
+    <mergeCell ref="H38:M38"/>
+    <mergeCell ref="N36:T36"/>
+    <mergeCell ref="U36:X36"/>
+    <mergeCell ref="N38:T38"/>
+    <mergeCell ref="U38:X38"/>
+    <mergeCell ref="Y36:AD36"/>
+    <mergeCell ref="U37:X37"/>
+    <mergeCell ref="Y38:AD38"/>
+    <mergeCell ref="Y41:AD41"/>
+    <mergeCell ref="C41:G41"/>
+    <mergeCell ref="H41:M41"/>
+    <mergeCell ref="N41:T41"/>
+    <mergeCell ref="U41:X41"/>
+    <mergeCell ref="Y40:AD40"/>
+    <mergeCell ref="C40:G40"/>
+    <mergeCell ref="H40:M40"/>
+    <mergeCell ref="N40:T40"/>
+    <mergeCell ref="U40:X40"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="H31:M31"/>
+    <mergeCell ref="N31:T31"/>
+    <mergeCell ref="U31:X31"/>
+    <mergeCell ref="Y31:AD31"/>
+    <mergeCell ref="Y34:AD34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="H35:M35"/>
+    <mergeCell ref="N35:T35"/>
+    <mergeCell ref="U35:X35"/>
+    <mergeCell ref="Y35:AD35"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="U34:X34"/>
+    <mergeCell ref="U33:X33"/>
+    <mergeCell ref="Y33:AD33"/>
+    <mergeCell ref="S29:Z29"/>
+    <mergeCell ref="AA29:AD29"/>
+    <mergeCell ref="U30:X30"/>
+    <mergeCell ref="Y30:AD30"/>
+    <mergeCell ref="U32:X32"/>
+    <mergeCell ref="Y32:AD32"/>
+    <mergeCell ref="A30:B43"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="H30:M30"/>
+    <mergeCell ref="N30:T30"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="H32:M32"/>
+    <mergeCell ref="N32:T32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="H33:M33"/>
+    <mergeCell ref="N33:T33"/>
+    <mergeCell ref="H34:M34"/>
+    <mergeCell ref="N34:T34"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="H37:M37"/>
+    <mergeCell ref="N37:T37"/>
+    <mergeCell ref="Y37:AD37"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="H36:M36"/>
+    <mergeCell ref="F24:J24"/>
+    <mergeCell ref="K24:N24"/>
+    <mergeCell ref="O24:R24"/>
+    <mergeCell ref="A28:B29"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="I28:L28"/>
+    <mergeCell ref="Y26:AD26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="F27:J27"/>
+    <mergeCell ref="K27:N27"/>
+    <mergeCell ref="O27:R27"/>
+    <mergeCell ref="Y27:AD27"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="F26:J26"/>
+    <mergeCell ref="K26:N26"/>
+    <mergeCell ref="O26:R26"/>
+    <mergeCell ref="M28:R28"/>
+    <mergeCell ref="S28:Z28"/>
+    <mergeCell ref="AA28:AD28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="I29:L29"/>
+    <mergeCell ref="M29:R29"/>
+    <mergeCell ref="K14:N14"/>
+    <mergeCell ref="O14:U14"/>
+    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="A14:B27"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="F14:J14"/>
+    <mergeCell ref="K22:N22"/>
+    <mergeCell ref="O22:R22"/>
+    <mergeCell ref="N13:T13"/>
+    <mergeCell ref="U13:AD13"/>
+    <mergeCell ref="Y22:AD22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="F23:J23"/>
+    <mergeCell ref="K23:N23"/>
+    <mergeCell ref="O23:R23"/>
+    <mergeCell ref="Y23:AD23"/>
+    <mergeCell ref="F22:J22"/>
+    <mergeCell ref="Y24:AD24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="F25:J25"/>
+    <mergeCell ref="K25:N25"/>
+    <mergeCell ref="O25:R25"/>
+    <mergeCell ref="Y25:AD25"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="AJ16:AK16"/>
+    <mergeCell ref="AV16:AX16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="F17:J17"/>
+    <mergeCell ref="K17:N17"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="F16:J16"/>
+    <mergeCell ref="K16:N16"/>
+    <mergeCell ref="O15:U15"/>
+    <mergeCell ref="O16:U16"/>
+    <mergeCell ref="O17:U17"/>
+    <mergeCell ref="V15:AD15"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="F15:J15"/>
+    <mergeCell ref="K15:N15"/>
+    <mergeCell ref="V17:AD17"/>
+    <mergeCell ref="V16:AD16"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="H1:AD2"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="K3:Q3"/>
+    <mergeCell ref="X3:Z3"/>
+    <mergeCell ref="T3:W3"/>
+    <mergeCell ref="K7:X7"/>
+    <mergeCell ref="AA8:AD8"/>
+    <mergeCell ref="Y6:AA6"/>
+    <mergeCell ref="AA3:AB3"/>
+    <mergeCell ref="AB6:AD6"/>
+    <mergeCell ref="Y7:AA7"/>
+    <mergeCell ref="AB7:AD7"/>
+    <mergeCell ref="AC3:AD3"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="K8:X8"/>
+    <mergeCell ref="P4:S4"/>
+    <mergeCell ref="AB5:AD5"/>
+    <mergeCell ref="P12:T12"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="F18:J18"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="F20:J20"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="O20:R20"/>
+    <mergeCell ref="Y20:AD20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="F21:J21"/>
+    <mergeCell ref="K21:N21"/>
+    <mergeCell ref="O21:R21"/>
+    <mergeCell ref="Y21:AD21"/>
+    <mergeCell ref="K20:N20"/>
+    <mergeCell ref="Y18:AD18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="F19:J19"/>
+    <mergeCell ref="K19:N19"/>
+    <mergeCell ref="O19:R19"/>
+    <mergeCell ref="Y19:AD19"/>
+    <mergeCell ref="K18:N18"/>
+    <mergeCell ref="O18:R18"/>
+    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="H13:M13"/>
     <mergeCell ref="U11:AD11"/>
     <mergeCell ref="A11:G11"/>
     <mergeCell ref="H12:M12"/>
@@ -9829,180 +10006,6 @@
     <mergeCell ref="V10:Z10"/>
     <mergeCell ref="U12:X12"/>
     <mergeCell ref="Y12:AD12"/>
-    <mergeCell ref="P12:T12"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="F18:J18"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="F20:J20"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="O20:R20"/>
-    <mergeCell ref="Y20:AD20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="F21:J21"/>
-    <mergeCell ref="K21:N21"/>
-    <mergeCell ref="O21:R21"/>
-    <mergeCell ref="Y21:AD21"/>
-    <mergeCell ref="K20:N20"/>
-    <mergeCell ref="Y18:AD18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="F19:J19"/>
-    <mergeCell ref="K19:N19"/>
-    <mergeCell ref="O19:R19"/>
-    <mergeCell ref="Y19:AD19"/>
-    <mergeCell ref="K18:N18"/>
-    <mergeCell ref="O18:R18"/>
-    <mergeCell ref="A13:G13"/>
-    <mergeCell ref="H13:M13"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="H1:AD2"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="K3:Q3"/>
-    <mergeCell ref="X3:Z3"/>
-    <mergeCell ref="T3:W3"/>
-    <mergeCell ref="K7:X7"/>
-    <mergeCell ref="AA8:AD8"/>
-    <mergeCell ref="Y6:AA6"/>
-    <mergeCell ref="AA3:AB3"/>
-    <mergeCell ref="AB6:AD6"/>
-    <mergeCell ref="Y7:AA7"/>
-    <mergeCell ref="AB7:AD7"/>
-    <mergeCell ref="AC3:AD3"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="K8:X8"/>
-    <mergeCell ref="P4:S4"/>
-    <mergeCell ref="AB5:AD5"/>
-    <mergeCell ref="AJ16:AK16"/>
-    <mergeCell ref="AV16:AX16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="F17:J17"/>
-    <mergeCell ref="K17:N17"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="F16:J16"/>
-    <mergeCell ref="K16:N16"/>
-    <mergeCell ref="O15:U15"/>
-    <mergeCell ref="O16:U16"/>
-    <mergeCell ref="O17:U17"/>
-    <mergeCell ref="V15:AD15"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="F15:J15"/>
-    <mergeCell ref="K15:N15"/>
-    <mergeCell ref="V17:AD17"/>
-    <mergeCell ref="V16:AD16"/>
-    <mergeCell ref="K14:N14"/>
-    <mergeCell ref="O14:U14"/>
-    <mergeCell ref="A12:G12"/>
-    <mergeCell ref="A14:B27"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="F14:J14"/>
-    <mergeCell ref="K22:N22"/>
-    <mergeCell ref="O22:R22"/>
-    <mergeCell ref="N13:T13"/>
-    <mergeCell ref="U13:AD13"/>
-    <mergeCell ref="Y22:AD22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="F23:J23"/>
-    <mergeCell ref="K23:N23"/>
-    <mergeCell ref="O23:R23"/>
-    <mergeCell ref="Y23:AD23"/>
-    <mergeCell ref="F22:J22"/>
-    <mergeCell ref="Y24:AD24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="F25:J25"/>
-    <mergeCell ref="K25:N25"/>
-    <mergeCell ref="O25:R25"/>
-    <mergeCell ref="Y25:AD25"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="F24:J24"/>
-    <mergeCell ref="K24:N24"/>
-    <mergeCell ref="O24:R24"/>
-    <mergeCell ref="A28:B29"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="I28:L28"/>
-    <mergeCell ref="Y26:AD26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="F27:J27"/>
-    <mergeCell ref="K27:N27"/>
-    <mergeCell ref="O27:R27"/>
-    <mergeCell ref="Y27:AD27"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="F26:J26"/>
-    <mergeCell ref="K26:N26"/>
-    <mergeCell ref="O26:R26"/>
-    <mergeCell ref="M28:R28"/>
-    <mergeCell ref="S28:Z28"/>
-    <mergeCell ref="AA28:AD28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="I29:L29"/>
-    <mergeCell ref="M29:R29"/>
-    <mergeCell ref="S29:Z29"/>
-    <mergeCell ref="AA29:AD29"/>
-    <mergeCell ref="U30:X30"/>
-    <mergeCell ref="Y30:AD30"/>
-    <mergeCell ref="U32:X32"/>
-    <mergeCell ref="Y32:AD32"/>
-    <mergeCell ref="A30:B43"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="H30:M30"/>
-    <mergeCell ref="N30:T30"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="H32:M32"/>
-    <mergeCell ref="N32:T32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="H33:M33"/>
-    <mergeCell ref="N33:T33"/>
-    <mergeCell ref="H34:M34"/>
-    <mergeCell ref="N34:T34"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="H37:M37"/>
-    <mergeCell ref="N37:T37"/>
-    <mergeCell ref="Y37:AD37"/>
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="H36:M36"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="H31:M31"/>
-    <mergeCell ref="N31:T31"/>
-    <mergeCell ref="U31:X31"/>
-    <mergeCell ref="Y31:AD31"/>
-    <mergeCell ref="Y34:AD34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="H35:M35"/>
-    <mergeCell ref="N35:T35"/>
-    <mergeCell ref="U35:X35"/>
-    <mergeCell ref="Y35:AD35"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="U34:X34"/>
-    <mergeCell ref="U33:X33"/>
-    <mergeCell ref="Y33:AD33"/>
-    <mergeCell ref="Y41:AD41"/>
-    <mergeCell ref="C41:G41"/>
-    <mergeCell ref="H41:M41"/>
-    <mergeCell ref="N41:T41"/>
-    <mergeCell ref="U41:X41"/>
-    <mergeCell ref="Y40:AD40"/>
-    <mergeCell ref="C40:G40"/>
-    <mergeCell ref="H40:M40"/>
-    <mergeCell ref="N40:T40"/>
-    <mergeCell ref="U40:X40"/>
-    <mergeCell ref="C39:G39"/>
-    <mergeCell ref="H39:M39"/>
-    <mergeCell ref="N39:T39"/>
-    <mergeCell ref="U39:X39"/>
-    <mergeCell ref="Y39:AD39"/>
-    <mergeCell ref="C38:G38"/>
-    <mergeCell ref="H38:M38"/>
-    <mergeCell ref="N36:T36"/>
-    <mergeCell ref="U36:X36"/>
-    <mergeCell ref="N38:T38"/>
-    <mergeCell ref="U38:X38"/>
-    <mergeCell ref="Y36:AD36"/>
-    <mergeCell ref="U37:X37"/>
-    <mergeCell ref="Y38:AD38"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <hyperlinks>
@@ -10046,64 +10049,64 @@
       <c r="B1" s="28"/>
     </row>
     <row r="3" spans="1:13" s="28" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A3" s="156" t="s">
+      <c r="A3" s="150" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="156"/>
-      <c r="C3" s="156"/>
-      <c r="D3" s="156"/>
-      <c r="E3" s="156"/>
-      <c r="F3" s="156"/>
-      <c r="G3" s="156"/>
-      <c r="H3" s="156"/>
-      <c r="I3" s="156"/>
-      <c r="J3" s="156"/>
-      <c r="K3" s="156"/>
-      <c r="L3" s="156"/>
+      <c r="B3" s="150"/>
+      <c r="C3" s="150"/>
+      <c r="D3" s="150"/>
+      <c r="E3" s="150"/>
+      <c r="F3" s="150"/>
+      <c r="G3" s="150"/>
+      <c r="H3" s="150"/>
+      <c r="I3" s="150"/>
+      <c r="J3" s="150"/>
+      <c r="K3" s="150"/>
+      <c r="L3" s="150"/>
     </row>
     <row r="5" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="157" t="s">
+      <c r="A5" s="151" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="I5" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="J5" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="K5" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="L5" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="M5" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="G5" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="H5" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="I5" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="J5" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="K5" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="L5" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="M5" s="31" t="s">
-        <v>64</v>
-      </c>
     </row>
     <row r="6" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="158"/>
+      <c r="A6" s="152"/>
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -10122,7 +10125,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="158"/>
+      <c r="A7" s="152"/>
       <c r="B7" s="29"/>
       <c r="C7" s="29"/>
       <c r="D7" s="29"/>
@@ -10137,7 +10140,7 @@
       <c r="M7" s="29"/>
     </row>
     <row r="8" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="158"/>
+      <c r="A8" s="152"/>
       <c r="B8" s="29"/>
       <c r="C8" s="29"/>
       <c r="D8" s="29"/>
@@ -10152,7 +10155,7 @@
       <c r="M8" s="29"/>
     </row>
     <row r="9" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="158"/>
+      <c r="A9" s="152"/>
       <c r="B9" s="29"/>
       <c r="C9" s="29"/>
       <c r="D9" s="29"/>
@@ -10167,7 +10170,7 @@
       <c r="M9" s="29"/>
     </row>
     <row r="10" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="158"/>
+      <c r="A10" s="152"/>
       <c r="B10" s="29"/>
       <c r="C10" s="29"/>
       <c r="D10" s="29"/>
@@ -10182,7 +10185,7 @@
       <c r="M10" s="29"/>
     </row>
     <row r="11" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="158"/>
+      <c r="A11" s="152"/>
       <c r="B11" s="29"/>
       <c r="C11" s="29"/>
       <c r="D11" s="29"/>
@@ -10197,7 +10200,7 @@
       <c r="M11" s="29"/>
     </row>
     <row r="12" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="158"/>
+      <c r="A12" s="152"/>
       <c r="B12" s="29"/>
       <c r="C12" s="29"/>
       <c r="D12" s="29"/>
@@ -10212,7 +10215,7 @@
       <c r="M12" s="29"/>
     </row>
     <row r="13" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="159"/>
+      <c r="A13" s="153"/>
       <c r="B13" s="32"/>
       <c r="C13" s="32"/>
       <c r="D13" s="32"/>
@@ -10227,103 +10230,108 @@
       <c r="M13" s="32"/>
     </row>
     <row r="19" spans="1:12" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="157" t="s">
+      <c r="A19" s="151" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="154" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="160" t="s">
+      <c r="C19" s="155"/>
+      <c r="D19" s="156"/>
+      <c r="E19" s="154" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="161"/>
-      <c r="D19" s="162"/>
-      <c r="E19" s="160" t="s">
+      <c r="F19" s="155"/>
+      <c r="G19" s="155"/>
+      <c r="H19" s="155"/>
+      <c r="I19" s="156"/>
+      <c r="J19" s="154" t="s">
         <v>45</v>
       </c>
-      <c r="F19" s="161"/>
-      <c r="G19" s="161"/>
-      <c r="H19" s="161"/>
-      <c r="I19" s="162"/>
-      <c r="J19" s="160" t="s">
-        <v>46</v>
-      </c>
-      <c r="K19" s="161" t="s">
+      <c r="K19" s="155" t="s">
+        <v>60</v>
+      </c>
+      <c r="L19" s="156" t="s">
         <v>61</v>
       </c>
-      <c r="L19" s="162" t="s">
-        <v>62</v>
-      </c>
     </row>
     <row r="20" spans="1:12" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="158"/>
-      <c r="B20" s="150"/>
-      <c r="C20" s="151"/>
-      <c r="D20" s="152"/>
-      <c r="E20" s="150"/>
-      <c r="F20" s="151"/>
-      <c r="G20" s="151"/>
-      <c r="H20" s="151"/>
-      <c r="I20" s="152"/>
-      <c r="J20" s="150"/>
-      <c r="K20" s="151"/>
-      <c r="L20" s="152"/>
+      <c r="A20" s="152"/>
+      <c r="B20" s="157"/>
+      <c r="C20" s="158"/>
+      <c r="D20" s="159"/>
+      <c r="E20" s="157"/>
+      <c r="F20" s="158"/>
+      <c r="G20" s="158"/>
+      <c r="H20" s="158"/>
+      <c r="I20" s="159"/>
+      <c r="J20" s="157"/>
+      <c r="K20" s="158"/>
+      <c r="L20" s="159"/>
     </row>
     <row r="21" spans="1:12" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="158"/>
-      <c r="B21" s="150"/>
-      <c r="C21" s="151"/>
-      <c r="D21" s="152"/>
-      <c r="E21" s="150"/>
-      <c r="F21" s="151"/>
-      <c r="G21" s="151"/>
-      <c r="H21" s="151"/>
-      <c r="I21" s="152"/>
-      <c r="J21" s="150"/>
-      <c r="K21" s="151"/>
-      <c r="L21" s="152"/>
+      <c r="A21" s="152"/>
+      <c r="B21" s="157"/>
+      <c r="C21" s="158"/>
+      <c r="D21" s="159"/>
+      <c r="E21" s="157"/>
+      <c r="F21" s="158"/>
+      <c r="G21" s="158"/>
+      <c r="H21" s="158"/>
+      <c r="I21" s="159"/>
+      <c r="J21" s="157"/>
+      <c r="K21" s="158"/>
+      <c r="L21" s="159"/>
     </row>
     <row r="22" spans="1:12" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="158"/>
-      <c r="B22" s="150"/>
-      <c r="C22" s="151"/>
-      <c r="D22" s="152"/>
-      <c r="E22" s="150"/>
-      <c r="F22" s="151"/>
-      <c r="G22" s="151"/>
-      <c r="H22" s="151"/>
-      <c r="I22" s="152"/>
-      <c r="J22" s="150"/>
-      <c r="K22" s="151"/>
-      <c r="L22" s="152"/>
+      <c r="A22" s="152"/>
+      <c r="B22" s="157"/>
+      <c r="C22" s="158"/>
+      <c r="D22" s="159"/>
+      <c r="E22" s="157"/>
+      <c r="F22" s="158"/>
+      <c r="G22" s="158"/>
+      <c r="H22" s="158"/>
+      <c r="I22" s="159"/>
+      <c r="J22" s="157"/>
+      <c r="K22" s="158"/>
+      <c r="L22" s="159"/>
     </row>
     <row r="23" spans="1:12" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="158"/>
-      <c r="B23" s="150"/>
-      <c r="C23" s="151"/>
-      <c r="D23" s="152"/>
-      <c r="E23" s="150"/>
-      <c r="F23" s="151"/>
-      <c r="G23" s="151"/>
-      <c r="H23" s="151"/>
-      <c r="I23" s="152"/>
-      <c r="J23" s="150"/>
-      <c r="K23" s="151"/>
-      <c r="L23" s="152"/>
+      <c r="A23" s="152"/>
+      <c r="B23" s="157"/>
+      <c r="C23" s="158"/>
+      <c r="D23" s="159"/>
+      <c r="E23" s="157"/>
+      <c r="F23" s="158"/>
+      <c r="G23" s="158"/>
+      <c r="H23" s="158"/>
+      <c r="I23" s="159"/>
+      <c r="J23" s="157"/>
+      <c r="K23" s="158"/>
+      <c r="L23" s="159"/>
     </row>
     <row r="24" spans="1:12" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="159"/>
-      <c r="B24" s="153"/>
-      <c r="C24" s="154"/>
-      <c r="D24" s="155"/>
-      <c r="E24" s="153"/>
-      <c r="F24" s="154"/>
-      <c r="G24" s="154"/>
-      <c r="H24" s="154"/>
-      <c r="I24" s="155"/>
-      <c r="J24" s="153"/>
-      <c r="K24" s="154"/>
-      <c r="L24" s="155"/>
+      <c r="A24" s="153"/>
+      <c r="B24" s="160"/>
+      <c r="C24" s="161"/>
+      <c r="D24" s="162"/>
+      <c r="E24" s="160"/>
+      <c r="F24" s="161"/>
+      <c r="G24" s="161"/>
+      <c r="H24" s="161"/>
+      <c r="I24" s="162"/>
+      <c r="J24" s="160"/>
+      <c r="K24" s="161"/>
+      <c r="L24" s="162"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="B22:D22"/>
     <mergeCell ref="A3:L3"/>
     <mergeCell ref="A5:A13"/>
     <mergeCell ref="A19:A24"/>
@@ -10340,11 +10348,6 @@
     <mergeCell ref="J23:L23"/>
     <mergeCell ref="E19:I19"/>
     <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="B22:D22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>